<commit_message>
Use DINS table to specify regional demand projections
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B7F3E-0C75-44BC-B299-44237A102472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97244D-5F3C-405C-A851-D0063DF7629B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="32" r:id="rId1"/>
@@ -928,7 +928,7 @@
     <t>Region</t>
   </si>
   <si>
-    <t>~TFM_INS</t>
+    <t>~TFM_DINS</t>
   </si>
 </sst>
 </file>
@@ -7881,8 +7881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D7C64-153E-41CE-9884-C520BAB2B293}">
   <dimension ref="B2:AF113"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20786,7 +20786,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:AK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update names of RSD demand commodities
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97244D-5F3C-405C-A851-D0063DF7629B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F41EC1-AB33-48EC-8274-3149A56B9048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="32" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="250">
   <si>
     <t>TimeSlice</t>
   </si>
@@ -902,27 +902,6 @@
   </si>
   <si>
     <t>Household occupancy rate</t>
-  </si>
-  <si>
-    <t>RSDRRF</t>
-  </si>
-  <si>
-    <t>RSDRCK</t>
-  </si>
-  <si>
-    <t>RSDRCW</t>
-  </si>
-  <si>
-    <t>RSDRCD</t>
-  </si>
-  <si>
-    <t>RSDRDW</t>
-  </si>
-  <si>
-    <t>RSDROE</t>
-  </si>
-  <si>
-    <t>RSDROA</t>
   </si>
   <si>
     <t>Region</t>
@@ -4842,7 +4821,7 @@
     </row>
     <row r="4" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -5523,7 +5502,7 @@
       </c>
       <c r="H15" s="36" t="str">
         <f>'BY-Demands'!I16</f>
-        <v>RSDRRF</v>
+        <v>RSDRF</v>
       </c>
       <c r="I15" s="6">
         <f>'BY-Demands'!J16</f>
@@ -5584,7 +5563,7 @@
       </c>
       <c r="H16" s="36" t="str">
         <f>'BY-Demands'!I17</f>
-        <v>RSDRCK</v>
+        <v>RSDCK</v>
       </c>
       <c r="I16" s="6">
         <f>'BY-Demands'!J17</f>
@@ -5645,7 +5624,7 @@
       </c>
       <c r="H17" s="36" t="str">
         <f>'BY-Demands'!I18</f>
-        <v>RSDRCW</v>
+        <v>RSDCW</v>
       </c>
       <c r="I17" s="6">
         <f>'BY-Demands'!J18</f>
@@ -5706,7 +5685,7 @@
       </c>
       <c r="H18" s="36" t="str">
         <f>'BY-Demands'!I19</f>
-        <v>RSDRCD</v>
+        <v>RSDCD</v>
       </c>
       <c r="I18" s="6">
         <f>'BY-Demands'!J19</f>
@@ -5767,7 +5746,7 @@
       </c>
       <c r="H19" s="36" t="str">
         <f>'BY-Demands'!I20</f>
-        <v>RSDRDW</v>
+        <v>RSDDW</v>
       </c>
       <c r="I19" s="6">
         <f>'BY-Demands'!J20</f>
@@ -5828,7 +5807,7 @@
       </c>
       <c r="H20" s="36" t="str">
         <f>'BY-Demands'!I21</f>
-        <v>RSDROE</v>
+        <v>RSDOE</v>
       </c>
       <c r="I20" s="6">
         <f>'BY-Demands'!J21</f>
@@ -5889,7 +5868,7 @@
       </c>
       <c r="H21" s="36" t="str">
         <f>'BY-Demands'!I22</f>
-        <v>RSDROA</v>
+        <v>RSDOA</v>
       </c>
       <c r="I21" s="6">
         <f>'BY-Demands'!J22</f>
@@ -7881,7 +7860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D7C64-153E-41CE-9884-C520BAB2B293}">
   <dimension ref="B2:AF113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7892,7 +7871,7 @@
   <sheetData>
     <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -20786,8 +20765,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:AK54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Y35" sqref="Y35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21936,7 +21915,7 @@
         <v>2018</v>
       </c>
       <c r="I16" t="s">
-        <v>248</v>
+        <v>46</v>
       </c>
       <c r="J16" s="30">
         <v>1.411707806586</v>
@@ -21959,7 +21938,7 @@
         <v>2018</v>
       </c>
       <c r="I17" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
       <c r="J17" s="30">
         <v>2.0517341103298801</v>
@@ -21982,7 +21961,7 @@
         <v>2018</v>
       </c>
       <c r="I18" t="s">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J18" s="30">
         <v>1.10232379053225</v>
@@ -22005,7 +21984,7 @@
         <v>2018</v>
       </c>
       <c r="I19" t="s">
-        <v>251</v>
+        <v>52</v>
       </c>
       <c r="J19" s="30">
         <v>1.7147299705762999</v>
@@ -22028,7 +22007,7 @@
         <v>2018</v>
       </c>
       <c r="I20" t="s">
-        <v>252</v>
+        <v>54</v>
       </c>
       <c r="J20" s="30">
         <v>1.1862012348846001</v>
@@ -22051,7 +22030,7 @@
         <v>2018</v>
       </c>
       <c r="I21" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="J21" s="30">
         <v>10.352794328441099</v>
@@ -22074,7 +22053,7 @@
         <v>2018</v>
       </c>
       <c r="I22" t="s">
-        <v>254</v>
+        <v>58</v>
       </c>
       <c r="J22" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Change TFGV to TRAF in multiple worksheets
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C95CA1A2-F143-47BA-8675-BA07384C2C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98ABED6-2372-47D3-9B30-03D3DEEDC135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12588" yWindow="720" windowWidth="10452" windowHeight="11640" tabRatio="766" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="32" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="256">
   <si>
     <t>TimeSlice</t>
   </si>
@@ -924,6 +924,9 @@
   <si>
     <t>~TFM_DINS</t>
   </si>
+  <si>
+    <t>TRAF</t>
+  </si>
 </sst>
 </file>
 
@@ -940,10 +943,17 @@
     <numFmt numFmtId="170" formatCode="0.0E+00"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1388,69 +1398,69 @@
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1461,19 +1471,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1482,24 +1492,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="20" borderId="3" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="20" borderId="3" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1512,7 +1522,7 @@
     <xf numFmtId="168" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1525,25 +1535,26 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="31" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="31" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="3" xfId="41" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="3" xfId="41" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41"/>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="41" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="13" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="13" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="13" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="19" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="19" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="41" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="13" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="3" xfId="41" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="3" xfId="41" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41"/>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="41" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="14" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="20" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="41" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="37" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="14" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="37" borderId="3" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3366,8 +3377,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AG20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4060,8 +4071,8 @@
       <c r="D10" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="81" t="s">
-        <v>30</v>
+      <c r="E10" s="93" t="s">
+        <v>255</v>
       </c>
       <c r="F10" s="81">
         <v>2018</v>
@@ -4155,7 +4166,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="87" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="F11" s="85">
         <v>2050</v>
@@ -4633,7 +4644,7 @@
   <dimension ref="A1:V57"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4934,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="I8" s="59">
         <f>TRA!F10</f>
@@ -7633,7 +7644,7 @@
       <c r="J57" s="20"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -7646,7 +7657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D7C64-153E-41CE-9884-C520BAB2B293}">
   <dimension ref="B2:AF102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -11615,7 +11626,7 @@
       </c>
       <c r="E37" s="63" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F37" s="63">
         <v>2020</v>
@@ -11731,7 +11742,7 @@
       </c>
       <c r="E38" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F38" s="64">
         <v>2025</v>
@@ -11847,7 +11858,7 @@
       </c>
       <c r="E39" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F39" s="64">
         <v>2030</v>
@@ -11963,7 +11974,7 @@
       </c>
       <c r="E40" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F40" s="64">
         <v>2035</v>
@@ -12079,7 +12090,7 @@
       </c>
       <c r="E41" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F41" s="64">
         <v>2040</v>
@@ -12195,7 +12206,7 @@
       </c>
       <c r="E42" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F42" s="64">
         <v>2045</v>
@@ -12311,7 +12322,7 @@
       </c>
       <c r="E43" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F43" s="64">
         <v>2050</v>
@@ -12427,7 +12438,7 @@
       </c>
       <c r="E44" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F44" s="64">
         <v>2055</v>
@@ -12543,7 +12554,7 @@
       </c>
       <c r="E45" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F45" s="64">
         <v>2060</v>
@@ -12659,7 +12670,7 @@
       </c>
       <c r="E46" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F46" s="64">
         <v>2065</v>
@@ -12775,7 +12786,7 @@
       </c>
       <c r="E47" s="64" t="str">
         <f>DEMANDS!$H$8</f>
-        <v>TFGV</v>
+        <v>TRAF</v>
       </c>
       <c r="F47" s="64">
         <v>2070</v>
@@ -19276,7 +19287,7 @@
   <dimension ref="C4:AK53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -19739,7 +19750,7 @@
         <v>2018</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="J9" s="30">
         <v>11.625551</v>
@@ -21107,7 +21118,7 @@
   <dimension ref="B2:T40"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -21396,7 +21407,7 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>31</v>
@@ -22167,7 +22178,7 @@
   </sheetPr>
   <dimension ref="C4:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Include new IND commodity names
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA75F405-A6CA-4EE4-9E59-41FA07027EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD05EF0-DBED-4862-9811-9F5E73FAA40E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="1935" windowWidth="10425" windowHeight="14355" tabRatio="766" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="32" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="239">
   <si>
     <t>TimeSlice</t>
   </si>
@@ -416,111 +416,6 @@
   </si>
   <si>
     <t>Wheat Demand</t>
-  </si>
-  <si>
-    <t>IIS</t>
-  </si>
-  <si>
-    <t>Iron and Steel Demand</t>
-  </si>
-  <si>
-    <t>Mt</t>
-  </si>
-  <si>
-    <t>IAL</t>
-  </si>
-  <si>
-    <t>Aluminium Demand</t>
-  </si>
-  <si>
-    <t>ICU</t>
-  </si>
-  <si>
-    <t>Copper Demand</t>
-  </si>
-  <si>
-    <t>INF</t>
-  </si>
-  <si>
-    <t>Other Non Ferrous Metals Demand</t>
-  </si>
-  <si>
-    <t>IAM</t>
-  </si>
-  <si>
-    <t>Ammonia Demand</t>
-  </si>
-  <si>
-    <t>ICL</t>
-  </si>
-  <si>
-    <t>Chlorine Demand</t>
-  </si>
-  <si>
-    <t>ICH</t>
-  </si>
-  <si>
-    <t>Other Chemicals Demand</t>
-  </si>
-  <si>
-    <t>ICM</t>
-  </si>
-  <si>
-    <t>Cement Demand</t>
-  </si>
-  <si>
-    <t>ILM</t>
-  </si>
-  <si>
-    <t>Lime Demand</t>
-  </si>
-  <si>
-    <t>IGH</t>
-  </si>
-  <si>
-    <t>Glass Hollow Demand</t>
-  </si>
-  <si>
-    <t>IGF</t>
-  </si>
-  <si>
-    <t>Glass Flat Demand</t>
-  </si>
-  <si>
-    <t>INM</t>
-  </si>
-  <si>
-    <t>Other Non Metallic Minerals Demand</t>
-  </si>
-  <si>
-    <t>IPH</t>
-  </si>
-  <si>
-    <t>High Quality Paper Demand</t>
-  </si>
-  <si>
-    <t>IPL</t>
-  </si>
-  <si>
-    <t>Low Quality Paper Demand</t>
-  </si>
-  <si>
-    <t>IOI</t>
-  </si>
-  <si>
-    <t>Other Industries</t>
-  </si>
-  <si>
-    <t>NEC</t>
-  </si>
-  <si>
-    <t>Non Energy Consumption - Chemicals</t>
-  </si>
-  <si>
-    <t>NEO</t>
-  </si>
-  <si>
-    <t>Non Energy Consumption - Others</t>
   </si>
   <si>
     <t>CHCS</t>
@@ -902,6 +797,84 @@
   </si>
   <si>
     <t>TRAF</t>
+  </si>
+  <si>
+    <t>INEM</t>
+  </si>
+  <si>
+    <t>IFAB</t>
+  </si>
+  <si>
+    <t>ITAP</t>
+  </si>
+  <si>
+    <t>IWAP</t>
+  </si>
+  <si>
+    <t>IPX4</t>
+  </si>
+  <si>
+    <t>ICAF</t>
+  </si>
+  <si>
+    <t>IRAP</t>
+  </si>
+  <si>
+    <t>IONM</t>
+  </si>
+  <si>
+    <t>IMAP</t>
+  </si>
+  <si>
+    <t>IMAE</t>
+  </si>
+  <si>
+    <t>IEOE</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>IOMA</t>
+  </si>
+  <si>
+    <t>Non-Energy Mining demand</t>
+  </si>
+  <si>
+    <t>Food and beverages demand</t>
+  </si>
+  <si>
+    <t>Textiles and textile products demand</t>
+  </si>
+  <si>
+    <t>Wood and wood products demand</t>
+  </si>
+  <si>
+    <t>Pulp, paper, publishing and printing demand</t>
+  </si>
+  <si>
+    <t>Chemicals and man-made fibres demand</t>
+  </si>
+  <si>
+    <t>Rubber and plastic products demand</t>
+  </si>
+  <si>
+    <t>Other non-metallic mineral products demand</t>
+  </si>
+  <si>
+    <t>Basic metals and fabricated metal products demand</t>
+  </si>
+  <si>
+    <t>Machinery and equipment n.e.c. demand</t>
+  </si>
+  <si>
+    <t>Electrical and optical equipment demand</t>
+  </si>
+  <si>
+    <t>Transport equipment manufacture demand</t>
+  </si>
+  <si>
+    <t>Other manufacturing demand</t>
   </si>
 </sst>
 </file>
@@ -2149,13 +2122,13 @@
     </row>
     <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="E5" s="42" t="str">
         <f>Regions!A11</f>
@@ -2264,7 +2237,7 @@
     </row>
     <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C6" s="42" t="str">
         <f>C5</f>
@@ -2381,7 +2354,7 @@
     </row>
     <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="C7" s="42" t="str">
         <f>"*"&amp;C5</f>
@@ -2498,223 +2471,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="46" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="46" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="46" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="46" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="46" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="46" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="46" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="46" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="46" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="46" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="46" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="46" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="46" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="46" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="46" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2758,13 +2731,16 @@
   <sheetPr codeName="Sheet9">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="C4:R21"/>
+  <dimension ref="C4:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C4" s="10" t="s">
@@ -2830,43 +2806,43 @@
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>92</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>227</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>97</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>228</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>99</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>229</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -2874,32 +2850,32 @@
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>230</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>232</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -2908,54 +2884,54 @@
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>107</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>234</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>235</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>115</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>237</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
@@ -2963,56 +2939,12 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3384,7 +3316,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="H3" s="50" t="str">
         <f>Regions!E$3</f>
@@ -3496,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="F4" s="81">
         <v>2018</v>
@@ -3588,7 +3520,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="86" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="F5" s="82">
         <v>2050</v>
@@ -3680,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F6" s="81">
         <v>2018</v>
@@ -3772,7 +3704,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="86" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F7" s="83">
         <v>2050</v>
@@ -3864,7 +3796,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="F8" s="81">
         <v>2018</v>
@@ -3956,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="86" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="F9" s="83">
         <v>2050</v>
@@ -4048,7 +3980,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="93" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="F10" s="81">
         <v>2018</v>
@@ -4142,7 +4074,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="87" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="F11" s="85">
         <v>2050</v>
@@ -4231,12 +4163,12 @@
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="41" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="49" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="C16" s="49">
         <v>2018</v>
@@ -4247,7 +4179,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="41" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="C17" s="41">
         <v>1</v>
@@ -4262,7 +4194,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="41" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="C18" s="41">
         <v>1</v>
@@ -4277,7 +4209,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="64" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="C19" s="64">
         <v>1</v>
@@ -4288,7 +4220,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="53" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C20" s="53">
         <v>1</v>
@@ -4497,7 +4429,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -4551,10 +4483,10 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="F10" s="40">
         <v>2.75</v>
@@ -4617,10 +4549,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4643,7 +4575,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4654,7 +4586,7 @@
     </row>
     <row r="4" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -4727,7 +4659,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="34" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="I5" s="58">
         <f>'BY-Demands'!J6</f>
@@ -4790,7 +4722,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="I6" s="59">
         <f>'BY-Demands'!J7</f>
@@ -4850,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="I7" s="59">
         <f>'BY-Demands'!J8</f>
@@ -4910,7 +4842,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="I8" s="59">
         <f>TRA!F10</f>
@@ -5279,51 +5211,51 @@
       </c>
       <c r="I14" s="6">
         <f>'BY-Demands'!J15</f>
-        <v>1.411707806586</v>
+        <v>0</v>
       </c>
       <c r="J14" s="51">
         <f t="shared" ref="J14:T14" si="5">I14*(1+$V$5)^(J$4-I$4)</f>
-        <v>1.4258601773470243</v>
+        <v>0</v>
       </c>
       <c r="K14" s="51">
         <f t="shared" si="5"/>
-        <v>1.4618649336105261</v>
+        <v>0</v>
       </c>
       <c r="L14" s="51">
         <f t="shared" si="5"/>
-        <v>1.4987788550882539</v>
+        <v>0</v>
       </c>
       <c r="M14" s="51">
         <f t="shared" si="5"/>
-        <v>1.5366248993411675</v>
+        <v>0</v>
       </c>
       <c r="N14" s="51">
         <f t="shared" si="5"/>
-        <v>1.5754266036374096</v>
+        <v>0</v>
       </c>
       <c r="O14" s="51">
         <f t="shared" si="5"/>
-        <v>1.6152080995906388</v>
+        <v>0</v>
       </c>
       <c r="P14" s="51">
         <f t="shared" si="5"/>
-        <v>1.6559941281679984</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="51">
         <f t="shared" si="5"/>
-        <v>1.6978100550770558</v>
+        <v>0</v>
       </c>
       <c r="R14" s="51">
         <f t="shared" si="5"/>
-        <v>1.740681886541281</v>
+        <v>0</v>
       </c>
       <c r="S14" s="51">
         <f t="shared" si="5"/>
-        <v>1.7846362854738755</v>
+        <v>0</v>
       </c>
       <c r="T14" s="51">
         <f t="shared" si="5"/>
-        <v>1.8297005880600117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -5340,51 +5272,51 @@
       </c>
       <c r="I15" s="6">
         <f>'BY-Demands'!J16</f>
-        <v>2.0517341103298801</v>
+        <v>0</v>
       </c>
       <c r="J15" s="51">
         <f t="shared" ref="J15:T15" si="6">I15*(1+$V$5)^(J$4-I$4)</f>
-        <v>2.0723027447859366</v>
+        <v>0</v>
       </c>
       <c r="K15" s="51">
         <f t="shared" si="6"/>
-        <v>2.1246309859526327</v>
+        <v>0</v>
       </c>
       <c r="L15" s="51">
         <f t="shared" si="6"/>
-        <v>2.1782805807827788</v>
+        <v>0</v>
       </c>
       <c r="M15" s="51">
         <f t="shared" si="6"/>
-        <v>2.233284895112202</v>
+        <v>0</v>
       </c>
       <c r="N15" s="51">
         <f t="shared" si="6"/>
-        <v>2.2896781373058963</v>
+        <v>0</v>
       </c>
       <c r="O15" s="51">
         <f t="shared" si="6"/>
-        <v>2.3474953795329392</v>
+        <v>0</v>
       </c>
       <c r="P15" s="51">
         <f t="shared" si="6"/>
-        <v>2.4067725795786274</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="51">
         <f t="shared" si="6"/>
-        <v>2.4675466032073956</v>
+        <v>0</v>
       </c>
       <c r="R15" s="51">
         <f t="shared" si="6"/>
-        <v>2.5298552470904285</v>
+        <v>0</v>
       </c>
       <c r="S15" s="51">
         <f t="shared" si="6"/>
-        <v>2.5937372623122221</v>
+        <v>0</v>
       </c>
       <c r="T15" s="51">
         <f t="shared" si="6"/>
-        <v>2.6592323784707159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -5401,51 +5333,51 @@
       </c>
       <c r="I16" s="6">
         <f>'BY-Demands'!J17</f>
-        <v>1.10232379053225</v>
+        <v>0</v>
       </c>
       <c r="J16" s="51">
         <f t="shared" ref="J16:T16" si="7">I16*(1+$V$5)^(J$4-I$4)</f>
-        <v>1.1133745865323355</v>
+        <v>0</v>
       </c>
       <c r="K16" s="51">
         <f t="shared" si="7"/>
-        <v>1.1414886900432841</v>
+        <v>0</v>
       </c>
       <c r="L16" s="51">
         <f t="shared" si="7"/>
-        <v>1.170312709898458</v>
+        <v>0</v>
       </c>
       <c r="M16" s="51">
         <f t="shared" si="7"/>
-        <v>1.1998645723751649</v>
+        <v>0</v>
       </c>
       <c r="N16" s="51">
         <f t="shared" si="7"/>
-        <v>1.2301626564116785</v>
+        <v>0</v>
       </c>
       <c r="O16" s="51">
         <f t="shared" si="7"/>
-        <v>1.2612258050374954</v>
+        <v>0</v>
       </c>
       <c r="P16" s="51">
         <f t="shared" si="7"/>
-        <v>1.2930733370922194</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="51">
         <f t="shared" si="7"/>
-        <v>1.3257250592403633</v>
+        <v>0</v>
       </c>
       <c r="R16" s="51">
         <f t="shared" si="7"/>
-        <v>1.3592012782895391</v>
+        <v>0</v>
       </c>
       <c r="S16" s="51">
         <f t="shared" si="7"/>
-        <v>1.3935228138196982</v>
+        <v>0</v>
       </c>
       <c r="T16" s="51">
         <f t="shared" si="7"/>
-        <v>1.4287110111312753</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
@@ -5462,51 +5394,51 @@
       </c>
       <c r="I17" s="6">
         <f>'BY-Demands'!J18</f>
-        <v>1.7147299705762999</v>
+        <v>0</v>
       </c>
       <c r="J17" s="51">
         <f t="shared" ref="J17:T17" si="8">I17*(1+$V$5)^(J$4-I$4)</f>
-        <v>1.731920138531327</v>
+        <v>0</v>
       </c>
       <c r="K17" s="51">
         <f t="shared" si="8"/>
-        <v>1.7756532923470774</v>
+        <v>0</v>
       </c>
       <c r="L17" s="51">
         <f t="shared" si="8"/>
-        <v>1.8204907630999205</v>
+        <v>0</v>
       </c>
       <c r="M17" s="51">
         <f t="shared" si="8"/>
-        <v>1.8664604361763686</v>
+        <v>0</v>
       </c>
       <c r="N17" s="51">
         <f t="shared" si="8"/>
-        <v>1.9135909011038872</v>
+        <v>0</v>
       </c>
       <c r="O17" s="51">
         <f t="shared" si="8"/>
-        <v>1.9619114693313366</v>
+        <v>0</v>
       </c>
       <c r="P17" s="51">
         <f t="shared" si="8"/>
-        <v>2.0114521924583921</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="51">
         <f t="shared" si="8"/>
-        <v>2.0622438809252794</v>
+        <v>0</v>
       </c>
       <c r="R17" s="51">
         <f t="shared" si="8"/>
-        <v>2.1143181231744488</v>
+        <v>0</v>
       </c>
       <c r="S17" s="51">
         <f t="shared" si="8"/>
-        <v>2.1677073052961071</v>
+        <v>0</v>
       </c>
       <c r="T17" s="51">
         <f t="shared" si="8"/>
-        <v>2.2224446311698229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
@@ -5523,51 +5455,51 @@
       </c>
       <c r="I18" s="6">
         <f>'BY-Demands'!J19</f>
-        <v>1.1862012348846001</v>
+        <v>0</v>
       </c>
       <c r="J18" s="51">
         <f t="shared" ref="J18:T18" si="9">I18*(1+$V$5)^(J$4-I$4)</f>
-        <v>1.1980929022643179</v>
+        <v>0</v>
       </c>
       <c r="K18" s="51">
         <f t="shared" si="9"/>
-        <v>1.2283462494104032</v>
+        <v>0</v>
       </c>
       <c r="L18" s="51">
         <f t="shared" si="9"/>
-        <v>1.2593635314832472</v>
+        <v>0</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="9"/>
-        <v>1.2911640387970591</v>
+        <v>0</v>
       </c>
       <c r="N18" s="51">
         <f t="shared" si="9"/>
-        <v>1.3237675487706548</v>
+        <v>0</v>
       </c>
       <c r="O18" s="51">
         <f t="shared" si="9"/>
-        <v>1.3571943382274592</v>
+        <v>0</v>
       </c>
       <c r="P18" s="51">
         <f t="shared" si="9"/>
-        <v>1.3914651960060977</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="51">
         <f t="shared" si="9"/>
-        <v>1.4266014358894226</v>
+        <v>0</v>
       </c>
       <c r="R18" s="51">
         <f t="shared" si="9"/>
-        <v>1.4626249098600117</v>
+        <v>0</v>
       </c>
       <c r="S18" s="51">
         <f t="shared" si="9"/>
-        <v>1.4995580216903865</v>
+        <v>0</v>
       </c>
       <c r="T18" s="51">
         <f t="shared" si="9"/>
-        <v>1.5374237408763995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
@@ -5584,51 +5516,51 @@
       </c>
       <c r="I19" s="6">
         <f>'BY-Demands'!J20</f>
-        <v>10.352794328441099</v>
+        <v>0</v>
       </c>
       <c r="J19" s="51">
         <f t="shared" ref="J19:T19" si="10">I19*(1+$V$5)^(J$4-I$4)</f>
-        <v>10.456581091583718</v>
+        <v>0</v>
       </c>
       <c r="K19" s="51">
         <f t="shared" si="10"/>
-        <v>10.720622867582055</v>
+        <v>0</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="10"/>
-        <v>10.991332029302525</v>
+        <v>0</v>
       </c>
       <c r="M19" s="51">
         <f t="shared" si="10"/>
-        <v>11.268876936589701</v>
+        <v>0</v>
       </c>
       <c r="N19" s="51">
         <f t="shared" si="10"/>
-        <v>11.553430200585208</v>
+        <v>0</v>
       </c>
       <c r="O19" s="51">
         <f t="shared" si="10"/>
-        <v>11.845168791078299</v>
+        <v>0</v>
       </c>
       <c r="P19" s="51">
         <f t="shared" si="10"/>
-        <v>12.144274146567174</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="51">
         <f t="shared" si="10"/>
-        <v>12.450932287099475</v>
+        <v>0</v>
       </c>
       <c r="R19" s="51">
         <f t="shared" si="10"/>
-        <v>12.765333929962157</v>
+        <v>0</v>
       </c>
       <c r="S19" s="51">
         <f t="shared" si="10"/>
-        <v>13.087674608292664</v>
+        <v>0</v>
       </c>
       <c r="T19" s="51">
         <f t="shared" si="10"/>
-        <v>13.418154792685185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
@@ -5892,7 +5824,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="I24" s="6">
         <f>'BY-Demands'!J25</f>
@@ -5952,7 +5884,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="I25" s="6">
         <f>'BY-Demands'!J26</f>
@@ -6012,7 +5944,7 @@
         <v>4</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="I26" s="6">
         <f>'BY-Demands'!J27</f>
@@ -6072,7 +6004,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="I27" s="6">
         <f>'BY-Demands'!J28</f>
@@ -6132,7 +6064,7 @@
         <v>4</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="I28" s="6">
         <f>'BY-Demands'!J29</f>
@@ -6192,7 +6124,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="I29" s="6">
         <f>'BY-Demands'!J30</f>
@@ -6252,7 +6184,7 @@
         <v>4</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="I30" s="6">
         <f>'BY-Demands'!J31</f>
@@ -6312,7 +6244,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="I31" s="6">
         <f>'BY-Demands'!J32</f>
@@ -6372,7 +6304,7 @@
         <v>4</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="I32" s="6">
         <f>'BY-Demands'!J33</f>
@@ -6432,7 +6364,7 @@
         <v>4</v>
       </c>
       <c r="H33" s="37" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="I33" s="6">
         <f>'BY-Demands'!J34</f>
@@ -6492,7 +6424,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="I34" s="6">
         <f>'BY-Demands'!J35</f>
@@ -6552,7 +6484,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="37" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="I35" s="6">
         <f>'BY-Demands'!J36</f>
@@ -6611,56 +6543,56 @@
       <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="38" t="s">
-        <v>92</v>
+      <c r="H36" s="41" t="s">
+        <v>213</v>
       </c>
       <c r="I36" s="6">
         <f>'BY-Demands'!J37</f>
-        <v>0</v>
+        <v>4.7617412851702303</v>
       </c>
       <c r="J36" s="39">
         <f t="shared" ref="J36:T36" si="27">I36*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>4.8094777415540602</v>
       </c>
       <c r="K36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>4.9309230814201204</v>
       </c>
       <c r="L36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.0554350683043694</v>
       </c>
       <c r="M36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.183091138886919</v>
       </c>
       <c r="N36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.31397068522109</v>
       </c>
       <c r="O36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.4481551041090395</v>
       </c>
       <c r="P36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.5857278477241783</v>
       </c>
       <c r="Q36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.7267744755118732</v>
       </c>
       <c r="R36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>5.8713827074007039</v>
       </c>
       <c r="S36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>6.0196424783573699</v>
       </c>
       <c r="T36" s="39">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>6.1716459943191806</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.2">
@@ -6671,56 +6603,56 @@
       <c r="E37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="38" t="s">
-        <v>95</v>
+      <c r="H37" s="41" t="s">
+        <v>214</v>
       </c>
       <c r="I37" s="6">
         <f>'BY-Demands'!J38</f>
-        <v>0</v>
+        <v>20.661699714695501</v>
       </c>
       <c r="J37" s="39">
         <f t="shared" ref="J37:T37" si="28">I37*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>20.868833254335318</v>
       </c>
       <c r="K37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>21.395797445329155</v>
       </c>
       <c r="L37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>21.936068142499234</v>
       </c>
       <c r="M37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>22.489981351801262</v>
       </c>
       <c r="N37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>23.057881563762386</v>
       </c>
       <c r="O37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>23.640121967727257</v>
       </c>
       <c r="P37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>24.237064671514066</v>
       </c>
       <c r="Q37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>24.849080926617184</v>
       </c>
       <c r="R37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>25.476551359096437</v>
       </c>
       <c r="S37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>26.119866206296635</v>
       </c>
       <c r="T37" s="39">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>26.779425559544567</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.2">
@@ -6731,56 +6663,56 @@
       <c r="E38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="38" t="s">
-        <v>97</v>
+      <c r="H38" s="41" t="s">
+        <v>215</v>
       </c>
       <c r="I38" s="6">
         <f>'BY-Demands'!J39</f>
-        <v>0</v>
+        <v>0.65822316983235796</v>
       </c>
       <c r="J38" s="39">
         <f t="shared" ref="J38:T38" si="29">I38*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>0.66482185710992714</v>
       </c>
       <c r="K38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.68160944210891949</v>
       </c>
       <c r="L38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.69882093466613127</v>
       </c>
       <c r="M38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.71646703897861808</v>
       </c>
       <c r="N38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.73455872953782475</v>
       </c>
       <c r="O38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.75310725795485767</v>
       </c>
       <c r="P38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.77212415995810324</v>
       </c>
       <c r="Q38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.7916212625675455</v>
       </c>
       <c r="R38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.81161069145024378</v>
       </c>
       <c r="S38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.83210487846154579</v>
       </c>
       <c r="T38" s="39">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.85311656937672531</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.2">
@@ -6791,56 +6723,56 @@
       <c r="E39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="38" t="s">
-        <v>99</v>
+      <c r="H39" s="41" t="s">
+        <v>216</v>
       </c>
       <c r="I39" s="6">
         <f>'BY-Demands'!J40</f>
-        <v>17.133327376888499</v>
+        <v>7.3077483223982496</v>
       </c>
       <c r="J39" s="51">
         <f t="shared" ref="J39:T39" si="30">I39*(1+$V$5)^(J$4-I$4)</f>
-        <v>17.305088983841802</v>
+        <v>7.3810084993302905</v>
       </c>
       <c r="K39" s="51">
         <f t="shared" si="30"/>
-        <v>17.742064166177503</v>
+        <v>7.5673882132877157</v>
       </c>
       <c r="L39" s="51">
         <f t="shared" si="30"/>
-        <v>18.190073519453072</v>
+        <v>7.7584742485802272</v>
       </c>
       <c r="M39" s="51">
         <f t="shared" si="30"/>
-        <v>18.649395670311971</v>
+        <v>7.9543854457191596</v>
       </c>
       <c r="N39" s="51">
         <f t="shared" si="30"/>
-        <v>19.120316281069563</v>
+        <v>8.1552436460876816</v>
       </c>
       <c r="O39" s="51">
         <f t="shared" si="30"/>
-        <v>19.603128227372643</v>
+        <v>8.3611737677165685</v>
       </c>
       <c r="P39" s="51">
         <f t="shared" si="30"/>
-        <v>20.098131780345106</v>
+        <v>8.5723038829734115</v>
       </c>
       <c r="Q39" s="51">
         <f t="shared" si="30"/>
-        <v>20.605634793332996</v>
+        <v>8.7887652982135744</v>
       </c>
       <c r="R39" s="51">
         <f t="shared" si="30"/>
-        <v>21.125952893365131</v>
+        <v>9.0106926354424388</v>
       </c>
       <c r="S39" s="51">
         <f t="shared" si="30"/>
-        <v>21.65940967744832</v>
+        <v>9.2382239160397202</v>
       </c>
       <c r="T39" s="51">
         <f t="shared" si="30"/>
-        <v>22.20633691381931</v>
+        <v>9.4715006465979297</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.2">
@@ -6851,56 +6783,56 @@
       <c r="E40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="38" t="s">
-        <v>101</v>
+      <c r="H40" s="41" t="s">
+        <v>217</v>
       </c>
       <c r="I40" s="6">
         <f>'BY-Demands'!J41</f>
-        <v>0</v>
+        <v>1.19344579337222</v>
       </c>
       <c r="J40" s="39">
         <f t="shared" ref="J40:T40" si="31">I40*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>1.2054100874507763</v>
       </c>
       <c r="K40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.23584820269219</v>
       </c>
       <c r="L40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.2670549184863078</v>
       </c>
       <c r="M40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.2990496429602403</v>
       </c>
       <c r="N40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.3318522743206287</v>
       </c>
       <c r="O40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.3654832132287666</v>
       </c>
       <c r="P40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.3999633754882106</v>
       </c>
       <c r="Q40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.4353142050527665</v>
       </c>
       <c r="R40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.4715576873629461</v>
       </c>
       <c r="S40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.5087163630191849</v>
       </c>
       <c r="T40" s="39">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1.5468133418003251</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.2">
@@ -6911,56 +6843,56 @@
       <c r="E41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H41" s="38" t="s">
-        <v>103</v>
+      <c r="H41" s="41" t="s">
+        <v>218</v>
       </c>
       <c r="I41" s="6">
         <f>'BY-Demands'!J42</f>
-        <v>0</v>
+        <v>11.2142608331669</v>
       </c>
       <c r="J41" s="39">
         <f t="shared" ref="J41:T41" si="32">I41*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>11.326683798019396</v>
       </c>
       <c r="K41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>11.612696757705406</v>
       </c>
       <c r="L41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>11.905931903034372</v>
       </c>
       <c r="M41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12.206571603244102</v>
       </c>
       <c r="N41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12.514802832624191</v>
       </c>
       <c r="O41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12.83081728679935</v>
       </c>
       <c r="P41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>13.154811501949032</v>
       </c>
       <c r="Q41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>13.486986977037507</v>
       </c>
       <c r="R41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>13.827550299130396</v>
       </c>
       <c r="S41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>14.176713271875606</v>
       </c>
       <c r="T41" s="39">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>14.534693047228574</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.2">
@@ -6971,56 +6903,56 @@
       <c r="E42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="38" t="s">
-        <v>105</v>
+      <c r="H42" s="41" t="s">
+        <v>219</v>
       </c>
       <c r="I42" s="6">
         <f>'BY-Demands'!J43</f>
-        <v>9.6435880892013799</v>
+        <v>2.3508165311810099</v>
       </c>
       <c r="J42" s="51">
         <f t="shared" ref="J42:T42" si="33">I42*(1+$V$5)^(J$4-I$4)</f>
-        <v>9.7402650597956217</v>
+        <v>2.374383466906099</v>
       </c>
       <c r="K42" s="51">
         <f t="shared" si="33"/>
-        <v>9.9862189583555452</v>
+        <v>2.434339624852178</v>
       </c>
       <c r="L42" s="51">
         <f t="shared" si="33"/>
-        <v>10.238383501065853</v>
+        <v>2.4958097509191433</v>
       </c>
       <c r="M42" s="51">
         <f t="shared" si="33"/>
-        <v>10.496915514474077</v>
+        <v>2.558832074699243</v>
       </c>
       <c r="N42" s="51">
         <f t="shared" si="33"/>
-        <v>10.761975785194595</v>
+        <v>2.6234457911298366</v>
       </c>
       <c r="O42" s="51">
         <f t="shared" si="33"/>
-        <v>11.033729159905286</v>
+        <v>2.6896910848695681</v>
       </c>
       <c r="P42" s="51">
         <f t="shared" si="33"/>
-        <v>11.312344647869219</v>
+        <v>2.7576091552900683</v>
       </c>
       <c r="Q42" s="51">
         <f t="shared" si="33"/>
-        <v>11.597995526045144</v>
+        <v>2.8272422420987304</v>
       </c>
       <c r="R42" s="51">
         <f t="shared" si="33"/>
-        <v>11.890859446852161</v>
+        <v>2.898633651608491</v>
       </c>
       <c r="S42" s="51">
         <f t="shared" si="33"/>
-        <v>12.191118548655572</v>
+        <v>2.9718277836709559</v>
       </c>
       <c r="T42" s="51">
         <f t="shared" si="33"/>
-        <v>12.498959569042643</v>
+        <v>3.0468701592896235</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.2">
@@ -7031,56 +6963,56 @@
       <c r="E43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="38" t="s">
-        <v>107</v>
+      <c r="H43" s="41" t="s">
+        <v>220</v>
       </c>
       <c r="I43" s="6">
         <f>'BY-Demands'!J44</f>
-        <v>4</v>
+        <v>19.0742645686014</v>
       </c>
       <c r="J43" s="51">
         <f t="shared" ref="J43:T43" si="34">I43*(1+$V$5)^(J$4-I$4)</f>
-        <v>4.0400999999999989</v>
+        <v>19.265484070901625</v>
       </c>
       <c r="K43" s="51">
         <f t="shared" si="34"/>
-        <v>4.1421175877629333</v>
+        <v>19.751961685811807</v>
       </c>
       <c r="L43" s="51">
         <f t="shared" si="34"/>
-        <v>4.2467112474579904</v>
+        <v>20.250723470117251</v>
       </c>
       <c r="M43" s="51">
         <f t="shared" si="34"/>
-        <v>4.3539460281296041</v>
+        <v>20.762079614488826</v>
       </c>
       <c r="N43" s="51">
         <f t="shared" si="34"/>
-        <v>4.4638886213920959</v>
+        <v>21.28634814230055</v>
       </c>
       <c r="O43" s="51">
         <f t="shared" si="34"/>
-        <v>4.576607402906621</v>
+        <v>21.823855107415156</v>
       </c>
       <c r="P43" s="51">
         <f t="shared" si="34"/>
-        <v>4.6921724749054627</v>
+        <v>22.374934796964002</v>
       </c>
       <c r="Q43" s="51">
         <f t="shared" si="34"/>
-        <v>4.810655709790117</v>
+        <v>22.939929939247413</v>
       </c>
       <c r="R43" s="51">
         <f t="shared" si="34"/>
-        <v>4.9321307948302833</v>
+        <v>23.519191916884783</v>
       </c>
       <c r="S43" s="51">
         <f t="shared" si="34"/>
-        <v>5.0566732779915586</v>
+        <v>24.113080985346972</v>
       </c>
       <c r="T43" s="51">
         <f t="shared" si="34"/>
-        <v>5.1843606149203447</v>
+        <v>24.721966497006925</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.2">
@@ -7091,56 +7023,56 @@
       <c r="E44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H44" s="38" t="s">
-        <v>109</v>
+      <c r="H44" s="41" t="s">
+        <v>221</v>
       </c>
       <c r="I44" s="6">
         <f>'BY-Demands'!J45</f>
-        <v>0.3</v>
+        <v>21.0459517518943</v>
       </c>
       <c r="J44" s="51">
         <f t="shared" ref="J44:T44" si="35">I44*(1+$V$5)^(J$4-I$4)</f>
-        <v>0.30300749999999993</v>
+        <v>21.256937418207034</v>
       </c>
       <c r="K44" s="51">
         <f t="shared" si="35"/>
-        <v>0.31065881908221998</v>
+        <v>21.793701725682872</v>
       </c>
       <c r="L44" s="51">
         <f t="shared" si="35"/>
-        <v>0.31850334355934923</v>
+        <v>22.344020004556928</v>
       </c>
       <c r="M44" s="51">
         <f t="shared" si="35"/>
-        <v>0.32654595210972026</v>
+        <v>22.908234509591864</v>
       </c>
       <c r="N44" s="51">
         <f t="shared" si="35"/>
-        <v>0.33479164660440713</v>
+        <v>23.486696137911999</v>
       </c>
       <c r="O44" s="51">
         <f t="shared" si="35"/>
-        <v>0.34324555521799649</v>
+        <v>24.079764647233752</v>
       </c>
       <c r="P44" s="51">
         <f t="shared" si="35"/>
-        <v>0.35191293561790965</v>
+        <v>24.687808879606706</v>
       </c>
       <c r="Q44" s="51">
         <f t="shared" si="35"/>
-        <v>0.36079917823425872</v>
+        <v>25.311206990804408</v>
       </c>
       <c r="R44" s="51">
         <f t="shared" si="35"/>
-        <v>0.36990980961227116</v>
+        <v>25.950346685507554</v>
       </c>
       <c r="S44" s="51">
         <f t="shared" si="35"/>
-        <v>0.37925049584936682</v>
+        <v>26.605625458425884</v>
       </c>
       <c r="T44" s="51">
         <f t="shared" si="35"/>
-        <v>0.3888270461190258</v>
+        <v>27.27745084150866</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.2">
@@ -7151,56 +7083,56 @@
       <c r="E45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H45" s="38" t="s">
-        <v>111</v>
+      <c r="H45" s="41" t="s">
+        <v>222</v>
       </c>
       <c r="I45" s="6">
         <f>'BY-Demands'!J46</f>
-        <v>0</v>
+        <v>1.4853180662205601</v>
       </c>
       <c r="J45" s="39">
         <f t="shared" ref="J45:T45" si="36">I45*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>1.5002083798344208</v>
       </c>
       <c r="K45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.5380905213785527</v>
       </c>
       <c r="L45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.5769292344678509</v>
       </c>
       <c r="M45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.6167486737325376</v>
       </c>
       <c r="N45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.6575736037375168</v>
       </c>
       <c r="O45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.6994294143839899</v>
       </c>
       <c r="P45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.7423421366999798</v>
       </c>
       <c r="Q45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.7863384590295877</v>
       </c>
       <c r="R45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.831445743631047</v>
       </c>
       <c r="S45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.8776920436939002</v>
       </c>
       <c r="T45" s="39">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1.9251061207858797</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.2">
@@ -7211,56 +7143,56 @@
       <c r="E46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="38" t="s">
-        <v>113</v>
+      <c r="H46" s="41" t="s">
+        <v>223</v>
       </c>
       <c r="I46" s="6">
         <f>'BY-Demands'!J47</f>
-        <v>0</v>
+        <v>12.237664953062801</v>
       </c>
       <c r="J46" s="39">
         <f t="shared" ref="J46:T46" si="37">I46*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>12.360347544217252</v>
       </c>
       <c r="K46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>12.672461808807869</v>
       </c>
       <c r="L46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>12.992457349698562</v>
       </c>
       <c r="M46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>13.320533178992157</v>
       </c>
       <c r="N46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>13.656893334096464</v>
       </c>
       <c r="O46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>14.001747004619526</v>
       </c>
       <c r="P46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>14.355308662469128</v>
       </c>
       <c r="Q46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>14.717798195237489</v>
       </c>
       <c r="R46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>15.089441042954078</v>
       </c>
       <c r="S46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>15.470468338291617</v>
       </c>
       <c r="T46" s="39">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>15.861117050312449</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.2">
@@ -7271,56 +7203,56 @@
       <c r="E47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="38" t="s">
-        <v>115</v>
+      <c r="H47" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="I47" s="6">
         <f>'BY-Demands'!J48</f>
-        <v>3.00326037480112</v>
+        <v>1.1240687136841201</v>
       </c>
       <c r="J47" s="51">
         <f t="shared" ref="J47:T47" si="38">I47*(1+$V$5)^(J$4-I$4)</f>
-        <v>3.0333680600585002</v>
+        <v>1.1353375025388031</v>
       </c>
       <c r="K47" s="51">
         <f t="shared" si="38"/>
-        <v>3.1099644047738044</v>
+        <v>1.1640061972012627</v>
       </c>
       <c r="L47" s="51">
         <f t="shared" si="38"/>
-        <v>3.1884949031782037</v>
+        <v>1.193398812329497</v>
       </c>
       <c r="M47" s="51">
         <f t="shared" si="38"/>
-        <v>3.2690083950760904</v>
+        <v>1.2235336278224318</v>
       </c>
       <c r="N47" s="51">
         <f t="shared" si="38"/>
-        <v>3.3515549535381197</v>
+        <v>1.254429385169348</v>
       </c>
       <c r="O47" s="51">
         <f t="shared" si="38"/>
-        <v>3.4361859160427293</v>
+        <v>1.2861052991056163</v>
       </c>
       <c r="P47" s="51">
         <f t="shared" si="38"/>
-        <v>3.5229539164040196</v>
+        <v>1.318581069562754</v>
       </c>
       <c r="Q47" s="51">
         <f t="shared" si="38"/>
-        <v>3.6119129175058537</v>
+        <v>1.3518768939202357</v>
       </c>
       <c r="R47" s="51">
         <f t="shared" si="38"/>
-        <v>3.7031182448625355</v>
+        <v>1.3860134795666779</v>
       </c>
       <c r="S47" s="51">
         <f t="shared" si="38"/>
-        <v>3.7966266210269342</v>
+        <v>1.4210120567782081</v>
       </c>
       <c r="T47" s="51">
         <f t="shared" si="38"/>
-        <v>3.89249620086746</v>
+        <v>1.456894391922031</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.2">
@@ -7331,301 +7263,61 @@
       <c r="E48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="38" t="s">
-        <v>117</v>
+      <c r="H48" s="41" t="s">
+        <v>225</v>
       </c>
       <c r="I48" s="6">
         <f>'BY-Demands'!J49</f>
-        <v>0.2</v>
+        <v>5.7797245324108504</v>
       </c>
       <c r="J48" s="51">
         <f t="shared" ref="J48:T48" si="39">I48*(1+$V$5)^(J$4-I$4)</f>
-        <v>0.20200499999999996</v>
+        <v>5.8376662708482678</v>
       </c>
       <c r="K48" s="51">
         <f t="shared" si="39"/>
-        <v>0.20710587938814667</v>
+        <v>5.9850746595309703</v>
       </c>
       <c r="L48" s="51">
         <f t="shared" si="39"/>
-        <v>0.21233556237289952</v>
+        <v>6.1362052947495087</v>
       </c>
       <c r="M48" s="51">
         <f t="shared" si="39"/>
-        <v>0.21769730140648019</v>
+        <v>6.2911521678933644</v>
       </c>
       <c r="N48" s="51">
         <f t="shared" si="39"/>
-        <v>0.22319443106960477</v>
+        <v>6.4500116437523864</v>
       </c>
       <c r="O48" s="51">
         <f t="shared" si="39"/>
-        <v>0.228830370145331</v>
+        <v>6.6128825204481263</v>
       </c>
       <c r="P48" s="51">
         <f t="shared" si="39"/>
-        <v>0.23460862374527311</v>
+        <v>6.7798660908785093</v>
       </c>
       <c r="Q48" s="51">
         <f t="shared" si="39"/>
-        <v>0.24053278548950585</v>
+        <v>6.951066205714068</v>
       </c>
       <c r="R48" s="51">
         <f t="shared" si="39"/>
-        <v>0.24660653974151414</v>
+        <v>7.1265893379849032</v>
       </c>
       <c r="S48" s="51">
         <f t="shared" si="39"/>
-        <v>0.2528336638995779</v>
+        <v>7.3065446492985506</v>
       </c>
       <c r="T48" s="51">
         <f t="shared" si="39"/>
-        <v>0.25921803074601718</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B49" s="41" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)="*","",Regions!$C$3),IF(LEFT(Regions!$D$3,1)="*","",Regions!$D$3))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H49" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="I49" s="6">
-        <f>'BY-Demands'!J50</f>
-        <v>0</v>
-      </c>
-      <c r="J49" s="39">
-        <f t="shared" ref="J49:T49" si="40">I49*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
-      </c>
-      <c r="K49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="L49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="M49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="O49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="P49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="Q49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="R49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="S49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="T49" s="39">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B50" s="41" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)="*","",Regions!$C$3),IF(LEFT(Regions!$D$3,1)="*","",Regions!$D$3))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="I50" s="6">
-        <f>'BY-Demands'!J51</f>
-        <v>47.590844488534202</v>
-      </c>
-      <c r="J50" s="51">
-        <f t="shared" ref="J50:T50" si="41">I50*(1+$V$5)^(J$4-I$4)</f>
-        <v>48.067942704531745</v>
-      </c>
-      <c r="K50" s="51">
-        <f t="shared" si="41"/>
-        <v>49.281718493112045</v>
-      </c>
-      <c r="L50" s="51">
-        <f t="shared" si="41"/>
-        <v>50.526143641370574</v>
-      </c>
-      <c r="M50" s="51">
-        <f t="shared" si="41"/>
-        <v>51.80199208404678</v>
-      </c>
-      <c r="N50" s="51">
-        <f t="shared" si="41"/>
-        <v>53.110057298702131</v>
-      </c>
-      <c r="O50" s="51">
-        <f t="shared" si="41"/>
-        <v>54.451152799200834</v>
-      </c>
-      <c r="P50" s="51">
-        <f t="shared" si="41"/>
-        <v>55.826112641651619</v>
-      </c>
-      <c r="Q50" s="51">
-        <f t="shared" si="41"/>
-        <v>57.235791943125136</v>
-      </c>
-      <c r="R50" s="51">
-        <f t="shared" si="41"/>
-        <v>58.681067413469641</v>
-      </c>
-      <c r="S50" s="51">
-        <f t="shared" si="41"/>
-        <v>60.162837900555679</v>
-      </c>
-      <c r="T50" s="51">
-        <f t="shared" si="41"/>
-        <v>61.682024949288909</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B51" s="41" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)="*","",Regions!$C$3),IF(LEFT(Regions!$D$3,1)="*","",Regions!$D$3))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H51" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="I51" s="6">
-        <f>'BY-Demands'!J52</f>
-        <v>0</v>
-      </c>
-      <c r="J51" s="39">
-        <f t="shared" ref="J51:T51" si="42">I51*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
-      </c>
-      <c r="K51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="L51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="O51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="P51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="R51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="S51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="T51" s="39">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B52" s="41" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)="*","",Regions!$C$3),IF(LEFT(Regions!$D$3,1)="*","",Regions!$D$3))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H52" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="I52" s="6">
-        <f>'BY-Demands'!J53</f>
-        <v>9.7255883662200109</v>
-      </c>
-      <c r="J52" s="51">
-        <f t="shared" ref="J52:T52" si="43">I52*(1+$V$5)^(J$4-I$4)</f>
-        <v>9.8230873895913646</v>
-      </c>
-      <c r="K52" s="51">
-        <f t="shared" si="43"/>
-        <v>10.07113265576562</v>
-      </c>
-      <c r="L52" s="51">
-        <f t="shared" si="43"/>
-        <v>10.325441375743274</v>
-      </c>
-      <c r="M52" s="51">
-        <f t="shared" si="43"/>
-        <v>10.586171709581775</v>
-      </c>
-      <c r="N52" s="51">
-        <f t="shared" si="43"/>
-        <v>10.853485811078212</v>
-      </c>
-      <c r="O52" s="51">
-        <f t="shared" si="43"/>
-        <v>11.127549928616251</v>
-      </c>
-      <c r="P52" s="51">
-        <f t="shared" si="43"/>
-        <v>11.40853450855958</v>
-      </c>
-      <c r="Q52" s="51">
-        <f t="shared" si="43"/>
-        <v>11.696614301256156</v>
-      </c>
-      <c r="R52" s="51">
-        <f t="shared" si="43"/>
-        <v>11.991968469719213</v>
-      </c>
-      <c r="S52" s="51">
-        <f t="shared" si="43"/>
-        <v>12.294780701052577</v>
-      </c>
-      <c r="T52" s="51">
-        <f t="shared" si="43"/>
-        <v>12.605239320689632</v>
-      </c>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I57" s="25"/>
-      <c r="J57" s="20"/>
+        <v>7.4910440577299298</v>
+      </c>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I53" s="25"/>
+      <c r="J53" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -7641,8 +7333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D7C64-153E-41CE-9884-C520BAB2B293}">
   <dimension ref="B2:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7652,7 +7344,7 @@
   <sheetData>
     <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -7669,7 +7361,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="G3" s="50" t="str">
         <f>Regions!E$3</f>
@@ -19268,10 +18960,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393D465E-96AD-44B8-AC1F-D38848D3C5B3}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="C4:AK53"/>
+  <dimension ref="C4:AK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19281,7 +18973,7 @@
   <sheetData>
     <row r="4" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C4" s="21" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -19291,10 +18983,10 @@
     </row>
     <row r="5" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="29" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>0</v>
@@ -19306,7 +18998,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>3</v>
@@ -19426,10 +19118,10 @@
     </row>
     <row r="6" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -19440,7 +19132,7 @@
         <v>2018</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="J6" s="30">
         <v>14.5565610923972</v>
@@ -19526,10 +19218,10 @@
     </row>
     <row r="7" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G7" s="28" t="s">
         <v>4</v>
@@ -19538,7 +19230,7 @@
         <v>2018</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="J7" s="30">
         <v>31.276118540281001</v>
@@ -19624,10 +19316,10 @@
     </row>
     <row r="8" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>4</v>
@@ -19636,7 +19328,7 @@
         <v>2018</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="J8" s="30">
         <v>27.131577542973599</v>
@@ -19722,10 +19414,10 @@
     </row>
     <row r="9" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G9" s="28" t="s">
         <v>4</v>
@@ -19734,7 +19426,7 @@
         <v>2018</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="J9" s="30">
         <v>11.625551</v>
@@ -19820,10 +19512,10 @@
     </row>
     <row r="10" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>4</v>
@@ -19918,10 +19610,10 @@
     </row>
     <row r="11" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G11" s="28" t="s">
         <v>4</v>
@@ -20016,10 +19708,10 @@
     </row>
     <row r="12" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G12" s="28" t="s">
         <v>4</v>
@@ -20114,10 +19806,10 @@
     </row>
     <row r="13" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>4</v>
@@ -20212,10 +19904,10 @@
     </row>
     <row r="14" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>4</v>
@@ -20311,10 +20003,10 @@
     </row>
     <row r="15" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G15" s="28" t="s">
         <v>4</v>
@@ -20325,19 +20017,14 @@
       <c r="I15" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="30">
-        <v>1.411707806586</v>
-      </c>
-      <c r="K15">
-        <v>1.411707806586</v>
-      </c>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G16" s="28" t="s">
         <v>4</v>
@@ -20348,19 +20035,14 @@
       <c r="I16" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="30">
-        <v>2.0517341103298801</v>
-      </c>
-      <c r="K16">
-        <v>2.0517341103298801</v>
-      </c>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>4</v>
@@ -20371,19 +20053,14 @@
       <c r="I17" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="30">
-        <v>1.10232379053225</v>
-      </c>
-      <c r="K17">
-        <v>1.10232379053225</v>
-      </c>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>4</v>
@@ -20394,19 +20071,14 @@
       <c r="I18" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="30">
-        <v>1.7147299705762999</v>
-      </c>
-      <c r="K18">
-        <v>1.7147299705762999</v>
-      </c>
+      <c r="J18" s="30"/>
     </row>
     <row r="19" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>4</v>
@@ -20417,19 +20089,14 @@
       <c r="I19" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="30">
-        <v>1.1862012348846001</v>
-      </c>
-      <c r="K19">
-        <v>1.1862012348846001</v>
-      </c>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G20" s="28" t="s">
         <v>4</v>
@@ -20440,19 +20107,14 @@
       <c r="I20" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="30">
-        <v>10.352794328441099</v>
-      </c>
-      <c r="K20">
-        <v>10.352794328441099</v>
-      </c>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G21" s="28" t="s">
         <v>4</v>
@@ -20463,19 +20125,14 @@
       <c r="I21" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="30">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G22" s="28" t="s">
         <v>4</v>
@@ -20495,10 +20152,10 @@
     </row>
     <row r="23" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>4</v>
@@ -20518,10 +20175,10 @@
     </row>
     <row r="24" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>4</v>
@@ -20541,10 +20198,10 @@
     </row>
     <row r="25" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>4</v>
@@ -20553,7 +20210,7 @@
         <v>2018</v>
       </c>
       <c r="I25" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="J25" s="30">
         <v>14.9399735840377</v>
@@ -20564,10 +20221,10 @@
     </row>
     <row r="26" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>4</v>
@@ -20576,7 +20233,7 @@
         <v>2018</v>
       </c>
       <c r="I26" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="J26" s="30">
         <v>12.334695394352201</v>
@@ -20587,10 +20244,10 @@
     </row>
     <row r="27" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G27" s="28" t="s">
         <v>4</v>
@@ -20599,7 +20256,7 @@
         <v>2018</v>
       </c>
       <c r="I27" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="J27" s="30">
         <v>5.9239600161508799</v>
@@ -20610,7 +20267,7 @@
     </row>
     <row r="28" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D28" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G28" s="28" t="s">
         <v>4</v>
@@ -20619,7 +20276,7 @@
         <v>2018</v>
       </c>
       <c r="I28" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="J28" s="30">
         <v>2.3392558619616</v>
@@ -20630,7 +20287,7 @@
     </row>
     <row r="29" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D29" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G29" s="28" t="s">
         <v>4</v>
@@ -20639,7 +20296,7 @@
         <v>2018</v>
       </c>
       <c r="I29" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="J29" s="30">
         <v>1.52795684913554</v>
@@ -20650,7 +20307,7 @@
     </row>
     <row r="30" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D30" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>4</v>
@@ -20659,7 +20316,7 @@
         <v>2018</v>
       </c>
       <c r="I30" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="J30" s="30">
         <v>1.32924900232905</v>
@@ -20670,7 +20327,7 @@
     </row>
     <row r="31" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D31" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>4</v>
@@ -20679,7 +20336,7 @@
         <v>2018</v>
       </c>
       <c r="I31" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="J31" s="30">
         <v>22.658222246043199</v>
@@ -20690,7 +20347,7 @@
     </row>
     <row r="32" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D32" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>4</v>
@@ -20699,7 +20356,7 @@
         <v>2018</v>
       </c>
       <c r="I32" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="J32" s="30">
         <v>1.0121675156415799</v>
@@ -20710,7 +20367,7 @@
     </row>
     <row r="33" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D33" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G33" s="28" t="s">
         <v>4</v>
@@ -20719,7 +20376,7 @@
         <v>2018</v>
       </c>
       <c r="I33" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="J33" s="30">
         <v>1.63362258706646</v>
@@ -20730,7 +20387,7 @@
     </row>
     <row r="34" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D34" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>4</v>
@@ -20739,7 +20396,7 @@
         <v>2018</v>
       </c>
       <c r="I34" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="J34" s="30">
         <v>0.62101142059626402</v>
@@ -20750,7 +20407,7 @@
     </row>
     <row r="35" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D35" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G35" s="28" t="s">
         <v>4</v>
@@ -20759,7 +20416,7 @@
         <v>2018</v>
       </c>
       <c r="I35" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="J35" s="30">
         <v>10.1146748592937</v>
@@ -20770,7 +20427,7 @@
     </row>
     <row r="36" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D36" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G36" s="28" t="s">
         <v>4</v>
@@ -20779,13 +20436,13 @@
         <v>2018</v>
       </c>
       <c r="I36" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="J36" s="31"/>
     </row>
     <row r="37" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D37" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G37" s="28" t="s">
         <v>4</v>
@@ -20794,13 +20451,18 @@
         <v>2018</v>
       </c>
       <c r="I37" t="s">
-        <v>92</v>
-      </c>
-      <c r="J37" s="31"/>
+        <v>213</v>
+      </c>
+      <c r="J37" s="31">
+        <v>4.7617412851702303</v>
+      </c>
+      <c r="K37">
+        <v>4.7617412851702303</v>
+      </c>
     </row>
     <row r="38" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D38" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>4</v>
@@ -20809,13 +20471,18 @@
         <v>2018</v>
       </c>
       <c r="I38" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="31"/>
+        <v>214</v>
+      </c>
+      <c r="J38" s="31">
+        <v>20.661699714695501</v>
+      </c>
+      <c r="K38">
+        <v>20.661699714695501</v>
+      </c>
     </row>
     <row r="39" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D39" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G39" s="28" t="s">
         <v>4</v>
@@ -20824,13 +20491,18 @@
         <v>2018</v>
       </c>
       <c r="I39" t="s">
-        <v>97</v>
-      </c>
-      <c r="J39" s="31"/>
+        <v>215</v>
+      </c>
+      <c r="J39" s="31">
+        <v>0.65822316983235796</v>
+      </c>
+      <c r="K39">
+        <v>0.65822316983235796</v>
+      </c>
     </row>
     <row r="40" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D40" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G40" s="28" t="s">
         <v>4</v>
@@ -20839,18 +20511,18 @@
         <v>2018</v>
       </c>
       <c r="I40" t="s">
-        <v>99</v>
+        <v>216</v>
       </c>
       <c r="J40" s="30">
-        <v>17.133327376888499</v>
+        <v>7.3077483223982496</v>
       </c>
       <c r="K40">
-        <v>17.133327376888499</v>
+        <v>7.3077483223982496</v>
       </c>
     </row>
     <row r="41" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D41" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>4</v>
@@ -20859,13 +20531,18 @@
         <v>2018</v>
       </c>
       <c r="I41" t="s">
-        <v>101</v>
-      </c>
-      <c r="J41" s="31"/>
+        <v>217</v>
+      </c>
+      <c r="J41" s="31">
+        <v>1.19344579337222</v>
+      </c>
+      <c r="K41">
+        <v>1.19344579337222</v>
+      </c>
     </row>
     <row r="42" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D42" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>4</v>
@@ -20874,13 +20551,18 @@
         <v>2018</v>
       </c>
       <c r="I42" t="s">
-        <v>103</v>
-      </c>
-      <c r="J42" s="31"/>
+        <v>218</v>
+      </c>
+      <c r="J42" s="31">
+        <v>11.2142608331669</v>
+      </c>
+      <c r="K42">
+        <v>11.2142608331669</v>
+      </c>
     </row>
     <row r="43" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D43" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G43" s="28" t="s">
         <v>4</v>
@@ -20889,18 +20571,18 @@
         <v>2018</v>
       </c>
       <c r="I43" t="s">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="J43" s="30">
-        <v>9.6435880892013799</v>
+        <v>2.3508165311810099</v>
       </c>
       <c r="K43">
-        <v>9.6435880892013799</v>
+        <v>2.3508165311810099</v>
       </c>
     </row>
     <row r="44" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D44" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G44" s="28" t="s">
         <v>4</v>
@@ -20909,18 +20591,18 @@
         <v>2018</v>
       </c>
       <c r="I44" t="s">
-        <v>107</v>
+        <v>220</v>
       </c>
       <c r="J44" s="30">
-        <v>4</v>
+        <v>19.0742645686014</v>
       </c>
       <c r="K44">
-        <v>4</v>
+        <v>19.0742645686014</v>
       </c>
     </row>
     <row r="45" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D45" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G45" s="28" t="s">
         <v>4</v>
@@ -20929,18 +20611,18 @@
         <v>2018</v>
       </c>
       <c r="I45" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="J45" s="30">
-        <v>0.3</v>
+        <v>21.0459517518943</v>
       </c>
       <c r="K45">
-        <v>0.3</v>
+        <v>21.0459517518943</v>
       </c>
     </row>
     <row r="46" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D46" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G46" s="28" t="s">
         <v>4</v>
@@ -20949,18 +20631,18 @@
         <v>2018</v>
       </c>
       <c r="I46" t="s">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="J46" s="30">
-        <v>0</v>
+        <v>1.4853180662205601</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>1.4853180662205601</v>
       </c>
     </row>
     <row r="47" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D47" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G47" s="28" t="s">
         <v>4</v>
@@ -20969,18 +20651,18 @@
         <v>2018</v>
       </c>
       <c r="I47" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="J47" s="30">
-        <v>0</v>
+        <v>12.237664953062801</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>12.237664953062801</v>
       </c>
     </row>
     <row r="48" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D48" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G48" s="28" t="s">
         <v>4</v>
@@ -20989,18 +20671,18 @@
         <v>2018</v>
       </c>
       <c r="I48" t="s">
-        <v>115</v>
+        <v>224</v>
       </c>
       <c r="J48" s="30">
-        <v>3.00326037480112</v>
+        <v>1.1240687136841201</v>
       </c>
       <c r="K48">
-        <v>3.00326037480112</v>
+        <v>1.1240687136841201</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D49" s="27" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G49" s="28" t="s">
         <v>4</v>
@@ -21009,83 +20691,13 @@
         <v>2018</v>
       </c>
       <c r="I49" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="J49" s="30">
-        <v>0.2</v>
+        <v>5.7797245324108504</v>
       </c>
       <c r="K49">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="50" spans="4:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="D50" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I50" t="s">
-        <v>119</v>
-      </c>
-      <c r="J50" s="31"/>
-    </row>
-    <row r="51" spans="4:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="D51" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G51" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H51" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I51" t="s">
-        <v>121</v>
-      </c>
-      <c r="J51" s="30">
-        <v>47.590844488534202</v>
-      </c>
-      <c r="K51">
-        <v>47.590844488534202</v>
-      </c>
-    </row>
-    <row r="52" spans="4:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="D52" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H52" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I52" t="s">
-        <v>123</v>
-      </c>
-      <c r="J52" s="31"/>
-    </row>
-    <row r="53" spans="4:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="D53" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H53" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I53" t="s">
-        <v>125</v>
-      </c>
-      <c r="J53" s="30">
-        <v>9.7255883662200109</v>
-      </c>
-      <c r="K53">
-        <v>9.7255883662200109</v>
+        <v>5.7797245324108504</v>
       </c>
     </row>
   </sheetData>
@@ -21197,10 +20809,10 @@
         <v>0.19950262849047029</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>41</v>
@@ -21263,10 +20875,10 @@
         <v>0.42864985886154994</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>41</v>
@@ -21329,10 +20941,10 @@
         <v>0.37184751264797972</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>41</v>
@@ -21391,13 +21003,13 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C10" s="13" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="F10" s="75">
         <f>COM_PROJ!G10</f>
@@ -21598,7 +21210,7 @@
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C19" s="8" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="F19" s="39">
         <v>53.674999999999997</v>
@@ -21642,7 +21254,7 @@
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C20" s="39" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="F20">
         <f>120/1000</f>
@@ -21699,7 +21311,7 @@
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C21" s="39" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="F21">
         <f>842*1.49/1000</f>
@@ -21756,7 +21368,7 @@
     </row>
     <row r="22" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C22" s="39" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="F22" s="39">
         <v>10.5185</v>
@@ -21800,7 +21412,7 @@
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C23" s="39" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="F23" s="39">
         <v>0.31718623699999998</v>
@@ -21856,7 +21468,7 @@
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C24" s="39" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="F24" s="39">
         <v>2.2810830000000002</v>
@@ -21912,7 +21524,7 @@
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C25" s="39" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="F25" s="39">
         <v>4.7131209901287638</v>
@@ -21968,7 +21580,7 @@
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C26" s="39" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="F26" s="39">
         <v>0.78552016502146071</v>
@@ -22024,7 +21636,7 @@
     </row>
     <row r="27" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="F27" s="9">
         <f>SUM(F19:F26)</f>
@@ -22081,7 +21693,7 @@
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C28" s="10" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="D28" s="39"/>
       <c r="F28" s="7">
@@ -22090,7 +21702,7 @@
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C29" s="10" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="D29" s="39"/>
       <c r="E29" s="39"/>
@@ -22100,7 +21712,7 @@
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C30" s="10" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="D30" s="39"/>
       <c r="E30" s="39"/>
@@ -22162,8 +21774,8 @@
   </sheetPr>
   <dimension ref="C4:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22849,7 +22461,7 @@
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C17" s="38" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="D17" s="38">
         <v>2017</v>
@@ -22896,7 +22508,7 @@
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C18" s="38" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="D18" s="55">
         <v>0.12384961999970633</v>
@@ -22943,7 +22555,7 @@
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C19" s="38" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="D19" s="55">
         <v>0.45119543431116133</v>
@@ -22990,7 +22602,7 @@
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C20" s="38" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="D20" s="55">
         <v>0.4249549456891325</v>
@@ -23125,10 +22737,10 @@
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
         <v>42</v>
@@ -23187,10 +22799,10 @@
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
@@ -23249,10 +22861,10 @@
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -23311,10 +22923,10 @@
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -23373,10 +22985,10 @@
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
@@ -23435,10 +23047,10 @@
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
@@ -23497,10 +23109,10 @@
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -23559,10 +23171,10 @@
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
@@ -23621,10 +23233,10 @@
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
@@ -23683,10 +23295,10 @@
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
         <v>42</v>
@@ -23745,10 +23357,10 @@
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
@@ -23807,10 +23419,10 @@
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
RSD: Enable non-architype demand and related stock in 2018
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1C3F72-3B6D-48E4-81A9-D9496F7C6CF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E5A463-0776-4768-AE66-BA5C31F814B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2355" yWindow="1860" windowWidth="20670" windowHeight="11385" tabRatio="766" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5211,51 +5211,51 @@
       </c>
       <c r="I14" s="6">
         <f>'BY-Demands'!J15</f>
-        <v>0</v>
+        <v>1.1293662452688</v>
       </c>
       <c r="J14" s="51">
         <f t="shared" ref="J14:T14" si="5">I14*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>1.1406881418776194</v>
       </c>
       <c r="K14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.1694919468884206</v>
       </c>
       <c r="L14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.1990230840706029</v>
       </c>
       <c r="M14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.2292999194729337</v>
       </c>
       <c r="N14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.2603412829099274</v>
       </c>
       <c r="O14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.2921664796725107</v>
       </c>
       <c r="P14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.3247953025343984</v>
       </c>
       <c r="Q14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.3582480440616442</v>
       </c>
       <c r="R14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.3925455092330243</v>
       </c>
       <c r="S14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.4277090283791001</v>
       </c>
       <c r="T14" s="51">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.4637604704480089</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -5272,51 +5272,51 @@
       </c>
       <c r="I15" s="6">
         <f>'BY-Demands'!J16</f>
-        <v>0</v>
+        <v>2.0006897535500099</v>
       </c>
       <c r="J15" s="51">
         <f t="shared" ref="J15:T15" si="6">I15*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>2.0207466683293482</v>
       </c>
       <c r="K15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.0717730539591463</v>
       </c>
       <c r="L15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.1240879197686957</v>
       </c>
       <c r="M15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.1777238014971658</v>
       </c>
       <c r="N15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.2327140564519117</v>
       </c>
       <c r="O15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.2890928842540998</v>
       </c>
       <c r="P15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.346895348108188</v>
       </c>
       <c r="Q15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.406157396608485</v>
       </c>
       <c r="R15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.4669158860963543</v>
       </c>
       <c r="S15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.5292086035819641</v>
       </c>
       <c r="T15" s="51">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.5930742902448416</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -5333,51 +5333,51 @@
       </c>
       <c r="I16" s="6">
         <f>'BY-Demands'!J17</f>
-        <v>0</v>
+        <v>0.77162665337257497</v>
       </c>
       <c r="J16" s="51">
         <f t="shared" ref="J16:T16" si="7">I16*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>0.77936221057263477</v>
       </c>
       <c r="K16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.79904208303029878</v>
       </c>
       <c r="L16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.81921889692892047</v>
       </c>
       <c r="M16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.83990520066261531</v>
       </c>
       <c r="N16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.86111385948817487</v>
       </c>
       <c r="O16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.88285806352624674</v>
       </c>
       <c r="P16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.90515133596455355</v>
       </c>
       <c r="Q16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.92800754146825426</v>
       </c>
       <c r="R16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.95144089480267735</v>
       </c>
       <c r="S16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.97546596967378874</v>
       </c>
       <c r="T16" s="51">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0000977077918927</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
@@ -5394,51 +5394,51 @@
       </c>
       <c r="I17" s="6">
         <f>'BY-Demands'!J18</f>
-        <v>0</v>
+        <v>1.0288379823457801</v>
       </c>
       <c r="J17" s="51">
         <f t="shared" ref="J17:T17" si="8">I17*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>1.0391520831187961</v>
       </c>
       <c r="K17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.0653919754082464</v>
       </c>
       <c r="L17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.0922944578599523</v>
       </c>
       <c r="M17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.1198762617058211</v>
       </c>
       <c r="N17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.1481545406623321</v>
       </c>
       <c r="O17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.1771468815988018</v>
       </c>
       <c r="P17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.206871315475035</v>
       </c>
       <c r="Q17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.2373463285551674</v>
       </c>
       <c r="R17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.268590873904669</v>
       </c>
       <c r="S17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.300624383177664</v>
       </c>
       <c r="T17" s="51">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.3334667787018937</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
@@ -5455,51 +5455,51 @@
       </c>
       <c r="I18" s="6">
         <f>'BY-Demands'!J19</f>
-        <v>0</v>
+        <v>0.83034086441921995</v>
       </c>
       <c r="J18" s="51">
         <f t="shared" ref="J18:T18" si="9">I18*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>0.83866503158502237</v>
       </c>
       <c r="K18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.85984237458728197</v>
       </c>
       <c r="L18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.88155447203827275</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.90381482715794104</v>
       </c>
       <c r="N18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.92663728413945801</v>
       </c>
       <c r="O18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.95003603675922099</v>
       </c>
       <c r="P18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.97402563720426794</v>
       </c>
       <c r="Q18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.99862100512259533</v>
       </c>
       <c r="R18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.0238374369020078</v>
       </c>
       <c r="S18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.0496906151832703</v>
       </c>
       <c r="T18" s="51">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.0761966186134795</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
@@ -5516,51 +5516,51 @@
       </c>
       <c r="I19" s="6">
         <f>'BY-Demands'!J20</f>
-        <v>0</v>
+        <v>9.2169270601308995</v>
       </c>
       <c r="J19" s="51">
         <f t="shared" ref="J19:T19" si="10">I19*(1+$V$5)^(J$4-I$4)</f>
-        <v>0</v>
+        <v>9.3093267539087083</v>
       </c>
       <c r="K19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>9.5443989202240758</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>9.7854069533144479</v>
       </c>
       <c r="M19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10.032500741254298</v>
       </c>
       <c r="N19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10.285833956979802</v>
       </c>
       <c r="O19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10.545564153861354</v>
       </c>
       <c r="P19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10.81185286368938</v>
       </c>
       <c r="Q19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>11.084865697134434</v>
       </c>
       <c r="R19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>11.364772446744036</v>
       </c>
       <c r="S19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>11.6517471925403</v>
       </c>
       <c r="T19" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>11.945968410284046</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
@@ -20017,7 +20017,12 @@
       <c r="I15" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="30">
+        <v>1.1293662452688</v>
+      </c>
+      <c r="K15">
+        <v>1.1293662452688</v>
+      </c>
     </row>
     <row r="16" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -20035,7 +20040,12 @@
       <c r="I16" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="30"/>
+      <c r="J16" s="30">
+        <v>2.0006897535500099</v>
+      </c>
+      <c r="K16">
+        <v>2.0006897535500099</v>
+      </c>
     </row>
     <row r="17" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
@@ -20053,7 +20063,12 @@
       <c r="I17" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="30"/>
+      <c r="J17" s="30">
+        <v>0.77162665337257497</v>
+      </c>
+      <c r="K17">
+        <v>0.77162665337257497</v>
+      </c>
     </row>
     <row r="18" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
@@ -20071,7 +20086,12 @@
       <c r="I18" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="30"/>
+      <c r="J18" s="30">
+        <v>1.0288379823457801</v>
+      </c>
+      <c r="K18">
+        <v>1.0288379823457801</v>
+      </c>
     </row>
     <row r="19" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -20089,7 +20109,12 @@
       <c r="I19" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="30"/>
+      <c r="J19" s="30">
+        <v>0.83034086441921995</v>
+      </c>
+      <c r="K19">
+        <v>0.83034086441921995</v>
+      </c>
     </row>
     <row r="20" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -20107,7 +20132,12 @@
       <c r="I20" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="30"/>
+      <c r="J20" s="30">
+        <v>9.2169270601308995</v>
+      </c>
+      <c r="K20">
+        <v>9.2169270601308995</v>
+      </c>
     </row>
     <row r="21" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -20125,7 +20155,12 @@
       <c r="I21" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="30"/>
+      <c r="J21" s="30">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">

</xml_diff>

<commit_message>
Convert RSD demand for m2 to the original units
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_Demands_BASE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A799D6-51A7-4254-83C5-4B58B104E4AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330B2076-9C14-4391-82B6-94CA1D55E5E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3135" yWindow="13380" windowWidth="20520" windowHeight="7800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="4" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="163">
   <si>
     <t>~TFM_INS-TS</t>
   </si>
@@ -1707,7 +1707,7 @@
   <dimension ref="C4:AK49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4469,8 +4469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935F79E2-0844-4822-9D59-D3ED84BB7C05}">
   <dimension ref="B2:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16863,10 +16863,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CL41"/>
+  <dimension ref="A1:CL52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CL28" sqref="CL28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16874,6 +16874,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:90" x14ac:dyDescent="0.25">
@@ -22304,109 +22305,144 @@
         <v>56</v>
       </c>
       <c r="H26">
-        <v>213414.55695615499</v>
+        <f>H50/1000</f>
+        <v>213.414556956155</v>
       </c>
       <c r="I26">
-        <v>218956.66937259401</v>
+        <f t="shared" ref="I26:AD28" si="0">I50/1000</f>
+        <v>218.95666937259401</v>
       </c>
       <c r="J26">
-        <v>225300.33816185399</v>
+        <f t="shared" si="0"/>
+        <v>225.30033816185397</v>
       </c>
       <c r="K26">
-        <v>242574.41637552099</v>
+        <f t="shared" si="0"/>
+        <v>242.574416375521</v>
       </c>
       <c r="L26">
-        <v>259561.94669652099</v>
+        <f t="shared" si="0"/>
+        <v>259.56194669652098</v>
       </c>
       <c r="M26">
-        <v>275023.94138045801</v>
+        <f t="shared" si="0"/>
+        <v>275.02394138045798</v>
       </c>
       <c r="N26">
-        <v>289113.78640676098</v>
+        <f t="shared" si="0"/>
+        <v>289.11378640676099</v>
       </c>
       <c r="O26">
-        <v>302217.18367944099</v>
+        <f t="shared" si="0"/>
+        <v>302.21718367944101</v>
       </c>
       <c r="P26">
-        <v>314549.61337722198</v>
+        <f t="shared" si="0"/>
+        <v>314.54961337722199</v>
       </c>
       <c r="Q26">
-        <v>326290.81316684798</v>
+        <f t="shared" si="0"/>
+        <v>326.29081316684795</v>
       </c>
       <c r="R26">
-        <v>337584.19698321301</v>
+        <f t="shared" si="0"/>
+        <v>337.58419698321302</v>
       </c>
       <c r="S26">
-        <v>348488.670477651</v>
+        <f t="shared" si="0"/>
+        <v>348.488670477651</v>
       </c>
       <c r="T26">
-        <v>359053.362495562</v>
+        <f t="shared" si="0"/>
+        <v>359.053362495562</v>
       </c>
       <c r="U26">
-        <v>379435.10129855498</v>
+        <f t="shared" si="0"/>
+        <v>379.43510129855497</v>
       </c>
       <c r="V26">
-        <v>394286.43020683102</v>
+        <f t="shared" si="0"/>
+        <v>394.28643020683103</v>
       </c>
       <c r="W26">
-        <v>409460.08200179902</v>
+        <f t="shared" si="0"/>
+        <v>409.46008200179904</v>
       </c>
       <c r="X26">
-        <v>424963.52313310798</v>
+        <f t="shared" si="0"/>
+        <v>424.96352313310797</v>
       </c>
       <c r="Y26">
-        <v>440776.66278306401</v>
+        <f t="shared" si="0"/>
+        <v>440.77666278306401</v>
       </c>
       <c r="Z26">
-        <v>456888.48985664902</v>
+        <f t="shared" si="0"/>
+        <v>456.88848985664902</v>
       </c>
       <c r="AA26">
-        <v>473286.23919771903</v>
+        <f t="shared" si="0"/>
+        <v>473.28623919771906</v>
       </c>
       <c r="AB26">
-        <v>489960.78944409703</v>
+        <f t="shared" si="0"/>
+        <v>489.96078944409703</v>
       </c>
       <c r="AC26">
-        <v>506886.30914768699</v>
+        <f t="shared" si="0"/>
+        <v>506.88630914768697</v>
       </c>
       <c r="AD26">
-        <v>524045.59801496298</v>
+        <f t="shared" si="0"/>
+        <v>524.04559801496293</v>
       </c>
       <c r="AI26">
-        <v>632981.68201128603</v>
+        <f t="shared" ref="AI26" si="1">AI50/1000</f>
+        <v>632.98168201128601</v>
       </c>
       <c r="AN26">
-        <v>740749.97310115199</v>
+        <f t="shared" ref="AN26" si="2">AN50/1000</f>
+        <v>740.74997310115202</v>
       </c>
       <c r="AS26">
-        <v>853983.36761178297</v>
+        <f t="shared" ref="AS26" si="3">AS50/1000</f>
+        <v>853.98336761178302</v>
       </c>
       <c r="AX26">
-        <v>973313.84240591305</v>
+        <f t="shared" ref="AX26" si="4">AX50/1000</f>
+        <v>973.31384240591308</v>
       </c>
       <c r="BC26">
-        <v>1101920.21948223</v>
+        <f t="shared" ref="BC26" si="5">BC50/1000</f>
+        <v>1101.9202194822301</v>
       </c>
       <c r="BH26">
-        <v>1243456.94226919</v>
+        <f t="shared" ref="BH26" si="6">BH50/1000</f>
+        <v>1243.45694226919</v>
       </c>
       <c r="BM26">
-        <v>1400399.1537987201</v>
+        <f t="shared" ref="BM26" si="7">BM50/1000</f>
+        <v>1400.3991537987201</v>
       </c>
       <c r="BR26">
-        <v>1574723.2584762699</v>
+        <f t="shared" ref="BR26" si="8">BR50/1000</f>
+        <v>1574.7232584762698</v>
       </c>
       <c r="BW26">
-        <v>1766492.4181818999</v>
+        <f t="shared" ref="BW26" si="9">BW50/1000</f>
+        <v>1766.4924181818999</v>
       </c>
       <c r="CB26">
-        <v>1974228.0679925601</v>
+        <f t="shared" ref="CB26" si="10">CB50/1000</f>
+        <v>1974.22806799256</v>
       </c>
       <c r="CG26">
-        <v>2195390.7432208802</v>
+        <f t="shared" ref="CG26" si="11">CG50/1000</f>
+        <v>2195.3907432208803</v>
       </c>
       <c r="CL26">
-        <v>2428365.4614147102</v>
+        <f t="shared" ref="CL26" si="12">CL50/1000</f>
+        <v>2428.3654614147104</v>
       </c>
     </row>
     <row r="27" spans="2:90" x14ac:dyDescent="0.25">
@@ -22424,109 +22460,144 @@
         <v>58</v>
       </c>
       <c r="H27">
-        <v>766617.95373000402</v>
+        <f t="shared" ref="H27:W28" si="13">H51/1000</f>
+        <v>766.61795373000405</v>
       </c>
       <c r="I27">
-        <v>776019.61867223098</v>
+        <f t="shared" si="13"/>
+        <v>776.01961867223099</v>
       </c>
       <c r="J27">
-        <v>788300.85620074603</v>
+        <f t="shared" si="13"/>
+        <v>788.30085620074601</v>
       </c>
       <c r="K27">
-        <v>801957.14588082698</v>
+        <f t="shared" si="13"/>
+        <v>801.95714588082694</v>
       </c>
       <c r="L27">
-        <v>819060.32622000796</v>
+        <f t="shared" si="13"/>
+        <v>819.06032622000794</v>
       </c>
       <c r="M27">
-        <v>834661.58347222698</v>
+        <f t="shared" si="13"/>
+        <v>834.66158347222699</v>
       </c>
       <c r="N27">
-        <v>848818.67768832797</v>
+        <f t="shared" si="13"/>
+        <v>848.81867768832797</v>
       </c>
       <c r="O27">
-        <v>862331.35320143297</v>
+        <f t="shared" si="13"/>
+        <v>862.33135320143299</v>
       </c>
       <c r="P27">
-        <v>875509.45116964797</v>
+        <f t="shared" si="13"/>
+        <v>875.50945116964795</v>
       </c>
       <c r="Q27">
-        <v>888595.96249835705</v>
+        <f t="shared" si="13"/>
+        <v>888.59596249835704</v>
       </c>
       <c r="R27">
-        <v>901764.69015385106</v>
+        <f t="shared" si="13"/>
+        <v>901.76469015385101</v>
       </c>
       <c r="S27">
-        <v>914993.375655549</v>
+        <f t="shared" si="13"/>
+        <v>914.99337565554902</v>
       </c>
       <c r="T27">
-        <v>928266.37631273095</v>
+        <f t="shared" si="13"/>
+        <v>928.26637631273093</v>
       </c>
       <c r="U27">
-        <v>943708.89277841605</v>
+        <f t="shared" si="13"/>
+        <v>943.70889277841604</v>
       </c>
       <c r="V27">
-        <v>957570.71779714397</v>
+        <f t="shared" si="13"/>
+        <v>957.57071779714397</v>
       </c>
       <c r="W27">
-        <v>971442.33945732203</v>
+        <f t="shared" si="13"/>
+        <v>971.44233945732208</v>
       </c>
       <c r="X27">
-        <v>985334.55511306797</v>
+        <f t="shared" si="0"/>
+        <v>985.33455511306795</v>
       </c>
       <c r="Y27">
-        <v>999194.66131792602</v>
+        <f t="shared" si="0"/>
+        <v>999.19466131792603</v>
       </c>
       <c r="Z27">
-        <v>1012994.63657764</v>
+        <f t="shared" si="0"/>
+        <v>1012.99463657764</v>
       </c>
       <c r="AA27">
-        <v>1026705.03546086</v>
+        <f t="shared" si="0"/>
+        <v>1026.70503546086</v>
       </c>
       <c r="AB27">
-        <v>1040306.63185868</v>
+        <f t="shared" si="0"/>
+        <v>1040.30663185868</v>
       </c>
       <c r="AC27">
-        <v>1053747.0705237</v>
+        <f t="shared" si="0"/>
+        <v>1053.7470705236999</v>
       </c>
       <c r="AD27">
-        <v>1066995.89427272</v>
+        <f t="shared" si="0"/>
+        <v>1066.9958942727201</v>
       </c>
       <c r="AI27">
-        <v>1166763.43459146</v>
+        <f t="shared" ref="AI27" si="14">AI51/1000</f>
+        <v>1166.7634345914601</v>
       </c>
       <c r="AN27">
-        <v>1244336.6649656901</v>
+        <f t="shared" ref="AN27" si="15">AN51/1000</f>
+        <v>1244.33666496569</v>
       </c>
       <c r="AS27">
-        <v>1314710.96966167</v>
+        <f t="shared" ref="AS27" si="16">AS51/1000</f>
+        <v>1314.7109696616701</v>
       </c>
       <c r="AX27">
-        <v>1379878.79642933</v>
+        <f t="shared" ref="AX27" si="17">AX51/1000</f>
+        <v>1379.8787964293301</v>
       </c>
       <c r="BC27">
-        <v>1444629.9926038501</v>
+        <f t="shared" ref="BC27" si="18">BC51/1000</f>
+        <v>1444.62999260385</v>
       </c>
       <c r="BH27">
-        <v>1512989.3882673399</v>
+        <f t="shared" ref="BH27" si="19">BH51/1000</f>
+        <v>1512.98938826734</v>
       </c>
       <c r="BM27">
-        <v>1586512.86397531</v>
+        <f t="shared" ref="BM27" si="20">BM51/1000</f>
+        <v>1586.51286397531</v>
       </c>
       <c r="BR27">
-        <v>1665745.9920316101</v>
+        <f t="shared" ref="BR27" si="21">BR51/1000</f>
+        <v>1665.7459920316101</v>
       </c>
       <c r="BW27">
-        <v>1749111.94897432</v>
+        <f t="shared" ref="BW27" si="22">BW51/1000</f>
+        <v>1749.1119489743201</v>
       </c>
       <c r="CB27">
-        <v>1833896.3857972301</v>
+        <f t="shared" ref="CB27" si="23">CB51/1000</f>
+        <v>1833.8963857972301</v>
       </c>
       <c r="CG27">
-        <v>1917030.21036523</v>
+        <f t="shared" ref="CG27" si="24">CG51/1000</f>
+        <v>1917.03021036523</v>
       </c>
       <c r="CL27">
-        <v>1996868.66239624</v>
+        <f t="shared" ref="CL27" si="25">CL51/1000</f>
+        <v>1996.8686623962401</v>
       </c>
     </row>
     <row r="28" spans="2:90" x14ac:dyDescent="0.25">
@@ -22544,109 +22615,144 @@
         <v>60</v>
       </c>
       <c r="H28">
-        <v>721105.90866437601</v>
+        <f t="shared" si="13"/>
+        <v>721.10590866437599</v>
       </c>
       <c r="I28">
-        <v>729040.47594293603</v>
+        <f t="shared" si="0"/>
+        <v>729.04047594293604</v>
       </c>
       <c r="J28">
-        <v>739683.68570912001</v>
+        <f t="shared" si="0"/>
+        <v>739.68368570912003</v>
       </c>
       <c r="K28">
-        <v>748342.44886999705</v>
+        <f t="shared" si="0"/>
+        <v>748.34244886999704</v>
       </c>
       <c r="L28">
-        <v>760630.721289968</v>
+        <f t="shared" si="0"/>
+        <v>760.63072128996805</v>
       </c>
       <c r="M28">
-        <v>771850.38797134894</v>
+        <f t="shared" si="0"/>
+        <v>771.85038797134894</v>
       </c>
       <c r="N28">
-        <v>782013.10939486197</v>
+        <f t="shared" si="0"/>
+        <v>782.013109394862</v>
       </c>
       <c r="O28">
-        <v>791820.47563049395</v>
+        <f t="shared" si="0"/>
+        <v>791.820475630494</v>
       </c>
       <c r="P28">
-        <v>801523.77429367404</v>
+        <f t="shared" si="0"/>
+        <v>801.52377429367402</v>
       </c>
       <c r="Q28">
-        <v>811316.73568663199</v>
+        <f t="shared" si="0"/>
+        <v>811.316735686632</v>
       </c>
       <c r="R28">
-        <v>821333.312278467</v>
+        <f t="shared" si="0"/>
+        <v>821.33331227846702</v>
       </c>
       <c r="S28">
-        <v>831532.33535063395</v>
+        <f t="shared" si="0"/>
+        <v>831.53233535063396</v>
       </c>
       <c r="T28">
-        <v>841882.469887482</v>
+        <f t="shared" si="0"/>
+        <v>841.88246988748199</v>
       </c>
       <c r="U28">
-        <v>851415.47129100398</v>
+        <f t="shared" si="0"/>
+        <v>851.415471291004</v>
       </c>
       <c r="V28">
-        <v>861039.36197674705</v>
+        <f t="shared" si="0"/>
+        <v>861.03936197674705</v>
       </c>
       <c r="W28">
-        <v>870573.18258039001</v>
+        <f t="shared" si="0"/>
+        <v>870.57318258039004</v>
       </c>
       <c r="X28">
-        <v>880025.70362676098</v>
+        <f t="shared" si="0"/>
+        <v>880.02570362676101</v>
       </c>
       <c r="Y28">
-        <v>889349.03440936899</v>
+        <f t="shared" si="0"/>
+        <v>889.34903440936898</v>
       </c>
       <c r="Z28">
-        <v>898517.81453963905</v>
+        <f t="shared" si="0"/>
+        <v>898.51781453963906</v>
       </c>
       <c r="AA28">
-        <v>907505.76600673597</v>
+        <f t="shared" si="0"/>
+        <v>907.50576600673594</v>
       </c>
       <c r="AB28">
-        <v>916295.97516395</v>
+        <f t="shared" si="0"/>
+        <v>916.29597516394995</v>
       </c>
       <c r="AC28">
-        <v>924842.69231704494</v>
+        <f t="shared" si="0"/>
+        <v>924.84269231704491</v>
       </c>
       <c r="AD28">
-        <v>933119.97808990802</v>
+        <f t="shared" si="0"/>
+        <v>933.11997808990805</v>
       </c>
       <c r="AI28">
-        <v>1001750.03116784</v>
+        <f t="shared" ref="AI28" si="26">AI52/1000</f>
+        <v>1001.75003116784</v>
       </c>
       <c r="AN28">
-        <v>1047946.93470063</v>
+        <f t="shared" ref="AN28" si="27">AN52/1000</f>
+        <v>1047.94693470063</v>
       </c>
       <c r="AS28">
-        <v>1085051.9905217399</v>
+        <f t="shared" ref="AS28" si="28">AS52/1000</f>
+        <v>1085.05199052174</v>
       </c>
       <c r="AX28">
-        <v>1114915.32706986</v>
+        <f t="shared" ref="AX28" si="29">AX52/1000</f>
+        <v>1114.91532706986</v>
       </c>
       <c r="BC28">
-        <v>1141469.10325923</v>
+        <f t="shared" ref="BC28" si="30">BC52/1000</f>
+        <v>1141.46910325923</v>
       </c>
       <c r="BH28">
-        <v>1167711.9675762199</v>
+        <f t="shared" ref="BH28" si="31">BH52/1000</f>
+        <v>1167.7119675762199</v>
       </c>
       <c r="BM28">
-        <v>1194473.05229634</v>
+        <f t="shared" ref="BM28" si="32">BM52/1000</f>
+        <v>1194.47305229634</v>
       </c>
       <c r="BR28">
-        <v>1221698.7321783099</v>
+        <f t="shared" ref="BR28" si="33">BR52/1000</f>
+        <v>1221.6987321783099</v>
       </c>
       <c r="BW28">
-        <v>1247749.8188300601</v>
+        <f t="shared" ref="BW28" si="34">BW52/1000</f>
+        <v>1247.7498188300601</v>
       </c>
       <c r="CB28">
-        <v>1270297.7134954601</v>
+        <f t="shared" ref="CB28" si="35">CB52/1000</f>
+        <v>1270.2977134954601</v>
       </c>
       <c r="CG28">
-        <v>1286979.0355445601</v>
+        <f t="shared" ref="CG28" si="36">CG52/1000</f>
+        <v>1286.97903554456</v>
       </c>
       <c r="CL28">
-        <v>1296606.1476706499</v>
+        <f t="shared" ref="CL28" si="37">CL52/1000</f>
+        <v>1296.60614767065</v>
       </c>
     </row>
     <row r="29" spans="2:90" x14ac:dyDescent="0.25">
@@ -23986,6 +24092,9 @@
       <c r="H40">
         <v>0</v>
       </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
       <c r="O40">
         <v>0</v>
       </c>
@@ -24033,6 +24142,602 @@
       </c>
       <c r="CL41">
         <v>32.865000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="6:90" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>87</v>
+      </c>
+      <c r="H49">
+        <v>2018</v>
+      </c>
+      <c r="I49">
+        <v>2019</v>
+      </c>
+      <c r="J49">
+        <v>2020</v>
+      </c>
+      <c r="K49">
+        <v>2021</v>
+      </c>
+      <c r="L49">
+        <v>2022</v>
+      </c>
+      <c r="M49">
+        <v>2023</v>
+      </c>
+      <c r="N49">
+        <v>2024</v>
+      </c>
+      <c r="O49">
+        <v>2025</v>
+      </c>
+      <c r="P49">
+        <v>2026</v>
+      </c>
+      <c r="Q49">
+        <v>2027</v>
+      </c>
+      <c r="R49">
+        <v>2028</v>
+      </c>
+      <c r="S49">
+        <v>2029</v>
+      </c>
+      <c r="T49">
+        <v>2030</v>
+      </c>
+      <c r="U49">
+        <v>2031</v>
+      </c>
+      <c r="V49">
+        <v>2032</v>
+      </c>
+      <c r="W49">
+        <v>2033</v>
+      </c>
+      <c r="X49">
+        <v>2034</v>
+      </c>
+      <c r="Y49">
+        <v>2035</v>
+      </c>
+      <c r="Z49">
+        <v>2036</v>
+      </c>
+      <c r="AA49">
+        <v>2037</v>
+      </c>
+      <c r="AB49">
+        <v>2038</v>
+      </c>
+      <c r="AC49">
+        <v>2039</v>
+      </c>
+      <c r="AD49">
+        <v>2040</v>
+      </c>
+      <c r="AE49">
+        <v>2041</v>
+      </c>
+      <c r="AF49">
+        <v>2042</v>
+      </c>
+      <c r="AG49">
+        <v>2043</v>
+      </c>
+      <c r="AH49">
+        <v>2044</v>
+      </c>
+      <c r="AI49">
+        <v>2045</v>
+      </c>
+      <c r="AJ49">
+        <v>2046</v>
+      </c>
+      <c r="AK49">
+        <v>2047</v>
+      </c>
+      <c r="AL49">
+        <v>2048</v>
+      </c>
+      <c r="AM49">
+        <v>2049</v>
+      </c>
+      <c r="AN49">
+        <v>2050</v>
+      </c>
+      <c r="AO49">
+        <v>2051</v>
+      </c>
+      <c r="AP49">
+        <v>2052</v>
+      </c>
+      <c r="AQ49">
+        <v>2053</v>
+      </c>
+      <c r="AR49">
+        <v>2054</v>
+      </c>
+      <c r="AS49">
+        <v>2055</v>
+      </c>
+      <c r="AT49">
+        <v>2056</v>
+      </c>
+      <c r="AU49">
+        <v>2057</v>
+      </c>
+      <c r="AV49">
+        <v>2058</v>
+      </c>
+      <c r="AW49">
+        <v>2059</v>
+      </c>
+      <c r="AX49">
+        <v>2060</v>
+      </c>
+      <c r="AY49">
+        <v>2061</v>
+      </c>
+      <c r="AZ49">
+        <v>2062</v>
+      </c>
+      <c r="BA49">
+        <v>2063</v>
+      </c>
+      <c r="BB49">
+        <v>2064</v>
+      </c>
+      <c r="BC49">
+        <v>2065</v>
+      </c>
+      <c r="BD49">
+        <v>2066</v>
+      </c>
+      <c r="BE49">
+        <v>2067</v>
+      </c>
+      <c r="BF49">
+        <v>2068</v>
+      </c>
+      <c r="BG49">
+        <v>2069</v>
+      </c>
+      <c r="BH49">
+        <v>2070</v>
+      </c>
+      <c r="BI49">
+        <v>2071</v>
+      </c>
+      <c r="BJ49">
+        <v>2072</v>
+      </c>
+      <c r="BK49">
+        <v>2073</v>
+      </c>
+      <c r="BL49">
+        <v>2074</v>
+      </c>
+      <c r="BM49">
+        <v>2075</v>
+      </c>
+      <c r="BN49">
+        <v>2076</v>
+      </c>
+      <c r="BO49">
+        <v>2077</v>
+      </c>
+      <c r="BP49">
+        <v>2078</v>
+      </c>
+      <c r="BQ49">
+        <v>2079</v>
+      </c>
+      <c r="BR49">
+        <v>2080</v>
+      </c>
+      <c r="BS49">
+        <v>2081</v>
+      </c>
+      <c r="BT49">
+        <v>2082</v>
+      </c>
+      <c r="BU49">
+        <v>2083</v>
+      </c>
+      <c r="BV49">
+        <v>2084</v>
+      </c>
+      <c r="BW49">
+        <v>2085</v>
+      </c>
+      <c r="BX49">
+        <v>2086</v>
+      </c>
+      <c r="BY49">
+        <v>2087</v>
+      </c>
+      <c r="BZ49">
+        <v>2088</v>
+      </c>
+      <c r="CA49">
+        <v>2089</v>
+      </c>
+      <c r="CB49">
+        <v>2090</v>
+      </c>
+      <c r="CC49">
+        <v>2091</v>
+      </c>
+      <c r="CD49">
+        <v>2092</v>
+      </c>
+      <c r="CE49">
+        <v>2093</v>
+      </c>
+      <c r="CF49">
+        <v>2094</v>
+      </c>
+      <c r="CG49">
+        <v>2095</v>
+      </c>
+      <c r="CH49">
+        <v>2096</v>
+      </c>
+      <c r="CI49">
+        <v>2097</v>
+      </c>
+      <c r="CJ49">
+        <v>2098</v>
+      </c>
+      <c r="CK49">
+        <v>2099</v>
+      </c>
+      <c r="CL49">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="50" spans="6:90" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" t="s">
+        <v>56</v>
+      </c>
+      <c r="H50">
+        <v>213414.55695615499</v>
+      </c>
+      <c r="I50">
+        <v>218956.66937259401</v>
+      </c>
+      <c r="J50">
+        <v>225300.33816185399</v>
+      </c>
+      <c r="K50">
+        <v>242574.41637552099</v>
+      </c>
+      <c r="L50">
+        <v>259561.94669652099</v>
+      </c>
+      <c r="M50">
+        <v>275023.94138045801</v>
+      </c>
+      <c r="N50">
+        <v>289113.78640676098</v>
+      </c>
+      <c r="O50">
+        <v>302217.18367944099</v>
+      </c>
+      <c r="P50">
+        <v>314549.61337722198</v>
+      </c>
+      <c r="Q50">
+        <v>326290.81316684798</v>
+      </c>
+      <c r="R50">
+        <v>337584.19698321301</v>
+      </c>
+      <c r="S50">
+        <v>348488.670477651</v>
+      </c>
+      <c r="T50">
+        <v>359053.362495562</v>
+      </c>
+      <c r="U50">
+        <v>379435.10129855498</v>
+      </c>
+      <c r="V50">
+        <v>394286.43020683102</v>
+      </c>
+      <c r="W50">
+        <v>409460.08200179902</v>
+      </c>
+      <c r="X50">
+        <v>424963.52313310798</v>
+      </c>
+      <c r="Y50">
+        <v>440776.66278306401</v>
+      </c>
+      <c r="Z50">
+        <v>456888.48985664902</v>
+      </c>
+      <c r="AA50">
+        <v>473286.23919771903</v>
+      </c>
+      <c r="AB50">
+        <v>489960.78944409703</v>
+      </c>
+      <c r="AC50">
+        <v>506886.30914768699</v>
+      </c>
+      <c r="AD50">
+        <v>524045.59801496298</v>
+      </c>
+      <c r="AI50">
+        <v>632981.68201128603</v>
+      </c>
+      <c r="AN50">
+        <v>740749.97310115199</v>
+      </c>
+      <c r="AS50">
+        <v>853983.36761178297</v>
+      </c>
+      <c r="AX50">
+        <v>973313.84240591305</v>
+      </c>
+      <c r="BC50">
+        <v>1101920.21948223</v>
+      </c>
+      <c r="BH50">
+        <v>1243456.94226919</v>
+      </c>
+      <c r="BM50">
+        <v>1400399.1537987201</v>
+      </c>
+      <c r="BR50">
+        <v>1574723.2584762699</v>
+      </c>
+      <c r="BW50">
+        <v>1766492.4181818999</v>
+      </c>
+      <c r="CB50">
+        <v>1974228.0679925601</v>
+      </c>
+      <c r="CG50">
+        <v>2195390.7432208802</v>
+      </c>
+      <c r="CL50">
+        <v>2428365.4614147102</v>
+      </c>
+    </row>
+    <row r="51" spans="6:90" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>57</v>
+      </c>
+      <c r="G51" t="s">
+        <v>58</v>
+      </c>
+      <c r="H51">
+        <v>766617.95373000402</v>
+      </c>
+      <c r="I51">
+        <v>776019.61867223098</v>
+      </c>
+      <c r="J51">
+        <v>788300.85620074603</v>
+      </c>
+      <c r="K51">
+        <v>801957.14588082698</v>
+      </c>
+      <c r="L51">
+        <v>819060.32622000796</v>
+      </c>
+      <c r="M51">
+        <v>834661.58347222698</v>
+      </c>
+      <c r="N51">
+        <v>848818.67768832797</v>
+      </c>
+      <c r="O51">
+        <v>862331.35320143297</v>
+      </c>
+      <c r="P51">
+        <v>875509.45116964797</v>
+      </c>
+      <c r="Q51">
+        <v>888595.96249835705</v>
+      </c>
+      <c r="R51">
+        <v>901764.69015385106</v>
+      </c>
+      <c r="S51">
+        <v>914993.375655549</v>
+      </c>
+      <c r="T51">
+        <v>928266.37631273095</v>
+      </c>
+      <c r="U51">
+        <v>943708.89277841605</v>
+      </c>
+      <c r="V51">
+        <v>957570.71779714397</v>
+      </c>
+      <c r="W51">
+        <v>971442.33945732203</v>
+      </c>
+      <c r="X51">
+        <v>985334.55511306797</v>
+      </c>
+      <c r="Y51">
+        <v>999194.66131792602</v>
+      </c>
+      <c r="Z51">
+        <v>1012994.63657764</v>
+      </c>
+      <c r="AA51">
+        <v>1026705.03546086</v>
+      </c>
+      <c r="AB51">
+        <v>1040306.63185868</v>
+      </c>
+      <c r="AC51">
+        <v>1053747.0705237</v>
+      </c>
+      <c r="AD51">
+        <v>1066995.89427272</v>
+      </c>
+      <c r="AI51">
+        <v>1166763.43459146</v>
+      </c>
+      <c r="AN51">
+        <v>1244336.6649656901</v>
+      </c>
+      <c r="AS51">
+        <v>1314710.96966167</v>
+      </c>
+      <c r="AX51">
+        <v>1379878.79642933</v>
+      </c>
+      <c r="BC51">
+        <v>1444629.9926038501</v>
+      </c>
+      <c r="BH51">
+        <v>1512989.3882673399</v>
+      </c>
+      <c r="BM51">
+        <v>1586512.86397531</v>
+      </c>
+      <c r="BR51">
+        <v>1665745.9920316101</v>
+      </c>
+      <c r="BW51">
+        <v>1749111.94897432</v>
+      </c>
+      <c r="CB51">
+        <v>1833896.3857972301</v>
+      </c>
+      <c r="CG51">
+        <v>1917030.21036523</v>
+      </c>
+      <c r="CL51">
+        <v>1996868.66239624</v>
+      </c>
+    </row>
+    <row r="52" spans="6:90" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52">
+        <v>721105.90866437601</v>
+      </c>
+      <c r="I52">
+        <v>729040.47594293603</v>
+      </c>
+      <c r="J52">
+        <v>739683.68570912001</v>
+      </c>
+      <c r="K52">
+        <v>748342.44886999705</v>
+      </c>
+      <c r="L52">
+        <v>760630.721289968</v>
+      </c>
+      <c r="M52">
+        <v>771850.38797134894</v>
+      </c>
+      <c r="N52">
+        <v>782013.10939486197</v>
+      </c>
+      <c r="O52">
+        <v>791820.47563049395</v>
+      </c>
+      <c r="P52">
+        <v>801523.77429367404</v>
+      </c>
+      <c r="Q52">
+        <v>811316.73568663199</v>
+      </c>
+      <c r="R52">
+        <v>821333.312278467</v>
+      </c>
+      <c r="S52">
+        <v>831532.33535063395</v>
+      </c>
+      <c r="T52">
+        <v>841882.469887482</v>
+      </c>
+      <c r="U52">
+        <v>851415.47129100398</v>
+      </c>
+      <c r="V52">
+        <v>861039.36197674705</v>
+      </c>
+      <c r="W52">
+        <v>870573.18258039001</v>
+      </c>
+      <c r="X52">
+        <v>880025.70362676098</v>
+      </c>
+      <c r="Y52">
+        <v>889349.03440936899</v>
+      </c>
+      <c r="Z52">
+        <v>898517.81453963905</v>
+      </c>
+      <c r="AA52">
+        <v>907505.76600673597</v>
+      </c>
+      <c r="AB52">
+        <v>916295.97516395</v>
+      </c>
+      <c r="AC52">
+        <v>924842.69231704494</v>
+      </c>
+      <c r="AD52">
+        <v>933119.97808990802</v>
+      </c>
+      <c r="AI52">
+        <v>1001750.03116784</v>
+      </c>
+      <c r="AN52">
+        <v>1047946.93470063</v>
+      </c>
+      <c r="AS52">
+        <v>1085051.9905217399</v>
+      </c>
+      <c r="AX52">
+        <v>1114915.32706986</v>
+      </c>
+      <c r="BC52">
+        <v>1141469.10325923</v>
+      </c>
+      <c r="BH52">
+        <v>1167711.9675762199</v>
+      </c>
+      <c r="BM52">
+        <v>1194473.05229634</v>
+      </c>
+      <c r="BR52">
+        <v>1221698.7321783099</v>
+      </c>
+      <c r="BW52">
+        <v>1247749.8188300601</v>
+      </c>
+      <c r="CB52">
+        <v>1270297.7134954601</v>
+      </c>
+      <c r="CG52">
+        <v>1286979.0355445601</v>
+      </c>
+      <c r="CL52">
+        <v>1296606.1476706499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>